<commit_message>
Split estimate hours sprint 2
</commit_message>
<xml_diff>
--- a/7.Print-Backlog/Sprint-2.xlsx
+++ b/7.Print-Backlog/Sprint-2.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Capstone1\7.Print-Backlog\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Actual" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="61">
   <si>
     <t>No</t>
   </si>
@@ -235,14 +230,11 @@
   <si>
     <t>Design Test Case for notification answer correct</t>
   </si>
-  <si>
-    <t>0,5</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
@@ -268,7 +260,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +282,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
@@ -424,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -521,8 +519,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -530,13 +537,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -557,7 +564,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -590,80 +597,75 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Actual!$G$36</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Estimate</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Actual!$H$1:$Z$1</c:f>
+              <c:f>Actual!$G$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>43393</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43394</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43395</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43396</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43397</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43398</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43399</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43400</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43401</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43402</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43403</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43404</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>43405</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>43406</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>43407</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>43408</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>43409</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>43410</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>43411</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>43412</c:v>
                 </c:pt>
               </c:numCache>
@@ -671,10 +673,164 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Actual!$H$36:$Z$36</c:f>
+              <c:f>Actual!$G$42:$Z$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2AF8-4A23-9267-01C3C33CDA35}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Actual!$G$1:$Z$1</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>43393</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43394</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43395</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43396</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43397</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43399</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43401</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43402</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43403</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43404</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43405</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>43406</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43407</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>43408</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43409</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43410</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43411</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43412</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Actual!$G$43:$Z$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -732,171 +888,13 @@
                 <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2AF8-4A23-9267-01C3C33CDA35}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Actual!$G$38</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Actual!$H$1:$Z$1</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>43394</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43395</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43396</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43397</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43398</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43399</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43400</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43401</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43402</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43403</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43404</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43405</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43406</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>43407</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>43408</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>43409</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>43410</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>43411</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>43412</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Actual!$H$38:$Z$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2AF8-4A23-9267-01C3C33CDA35}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -906,12 +904,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="195147648"/>
-        <c:axId val="195149184"/>
+        <c:axId val="207074816"/>
+        <c:axId val="207076352"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="195147648"/>
+        <c:axId val="207074816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -921,14 +920,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195149184"/>
+        <c:crossAx val="207076352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="195149184"/>
+        <c:axId val="207076352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,13 +938,23 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="195147648"/>
+        <c:crossAx val="207074816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.91379355105176174"/>
+          <c:y val="0.3660860757587015"/>
+          <c:w val="8.0229928204103365E-2"/>
+          <c:h val="0.1804079975009075"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -965,15 +974,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>326570</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>163285</xdr:rowOff>
+      <xdr:colOff>1129393</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>544285</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>149678</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>462644</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>176892</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1038,7 +1047,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1073,7 +1082,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1284,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,15 +1421,15 @@
         <v>5</v>
       </c>
       <c r="E2" s="21">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G2" s="23">
-        <v>0</v>
-      </c>
-      <c r="H2" s="23">
+        <v>1</v>
+      </c>
+      <c r="H2" s="42">
         <v>0</v>
       </c>
       <c r="I2" s="23">
@@ -1485,7 +1494,7 @@
       <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="35" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -1498,15 +1507,15 @@
         <v>4</v>
       </c>
       <c r="F3" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G3" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H3" s="23">
-        <v>0</v>
-      </c>
-      <c r="I3" s="23">
+        <v>1</v>
+      </c>
+      <c r="I3" s="42">
         <v>0</v>
       </c>
       <c r="J3" s="23">
@@ -1568,7 +1577,7 @@
       <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="16" t="s">
         <v>20</v>
       </c>
@@ -1576,21 +1585,21 @@
         <v>6</v>
       </c>
       <c r="E4" s="27">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I4" s="23">
-        <v>0</v>
-      </c>
-      <c r="J4" s="23">
+        <v>3</v>
+      </c>
+      <c r="J4" s="42">
         <v>0</v>
       </c>
       <c r="K4" s="23">
@@ -1649,7 +1658,7 @@
       <c r="A5" s="26">
         <v>4</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="35" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="29" t="s">
@@ -1658,25 +1667,25 @@
       <c r="D5" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="27" t="s">
-        <v>61</v>
+      <c r="E5" s="27">
+        <v>1</v>
       </c>
       <c r="F5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="23">
-        <v>0</v>
-      </c>
-      <c r="J5" s="23">
-        <v>0</v>
-      </c>
-      <c r="K5" s="23">
+        <v>1</v>
+      </c>
+      <c r="J5" s="42">
+        <v>0</v>
+      </c>
+      <c r="K5" s="42">
         <v>0</v>
       </c>
       <c r="L5" s="23">
@@ -1732,7 +1741,7 @@
       <c r="A6" s="26">
         <v>5</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="13" t="s">
         <v>14</v>
       </c>
@@ -1740,27 +1749,27 @@
         <v>5</v>
       </c>
       <c r="E6" s="27">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K6" s="23">
-        <v>0</v>
-      </c>
-      <c r="L6" s="23">
+        <v>4</v>
+      </c>
+      <c r="L6" s="42">
         <v>0</v>
       </c>
       <c r="M6" s="23">
@@ -1813,7 +1822,7 @@
       <c r="A7" s="26">
         <v>6</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="35" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -1822,31 +1831,31 @@
       <c r="D7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="27" t="s">
-        <v>61</v>
+      <c r="E7" s="33">
+        <v>0.5</v>
       </c>
       <c r="F7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L7" s="23">
-        <v>0</v>
-      </c>
-      <c r="M7" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M7" s="42">
         <v>0</v>
       </c>
       <c r="N7" s="23">
@@ -1907,27 +1916,27 @@
         <v>1</v>
       </c>
       <c r="F8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="23">
-        <v>0</v>
-      </c>
-      <c r="M8" s="23">
+        <v>1</v>
+      </c>
+      <c r="M8" s="42">
         <v>0</v>
       </c>
       <c r="N8" s="23">
@@ -1977,7 +1986,7 @@
       <c r="A9" s="26">
         <v>8</v>
       </c>
-      <c r="B9" s="38"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="13" t="s">
         <v>15</v>
       </c>
@@ -1988,27 +1997,27 @@
         <v>1</v>
       </c>
       <c r="F9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="23">
-        <v>0</v>
-      </c>
-      <c r="M9" s="23">
+        <v>1</v>
+      </c>
+      <c r="M9" s="42">
         <v>0</v>
       </c>
       <c r="N9" s="23">
@@ -2058,7 +2067,7 @@
       <c r="A10" s="26">
         <v>9</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="35" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -2067,31 +2076,31 @@
       <c r="D10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="27" t="s">
-        <v>61</v>
+      <c r="E10" s="33">
+        <v>0.5</v>
       </c>
       <c r="F10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L10" s="23">
-        <v>0</v>
-      </c>
-      <c r="M10" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="42">
         <v>0</v>
       </c>
       <c r="N10" s="23">
@@ -2152,30 +2161,30 @@
         <v>4</v>
       </c>
       <c r="F11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M11" s="23">
-        <v>0</v>
-      </c>
-      <c r="N11" s="23">
+        <v>3</v>
+      </c>
+      <c r="N11" s="42">
         <v>0</v>
       </c>
       <c r="O11" s="23">
@@ -2233,33 +2242,33 @@
         <v>2</v>
       </c>
       <c r="F12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N12" s="23">
-        <v>0</v>
-      </c>
-      <c r="O12" s="23">
+        <v>1</v>
+      </c>
+      <c r="O12" s="42">
         <v>0</v>
       </c>
       <c r="P12" s="23">
@@ -2303,7 +2312,7 @@
       <c r="A13" s="26">
         <v>12</v>
       </c>
-      <c r="B13" s="38"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="17" t="s">
         <v>31</v>
       </c>
@@ -2314,36 +2323,36 @@
         <v>4</v>
       </c>
       <c r="F13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O13" s="23">
-        <v>0</v>
-      </c>
-      <c r="P13" s="23">
+        <v>1</v>
+      </c>
+      <c r="P13" s="42">
         <v>0</v>
       </c>
       <c r="Q13" s="23">
@@ -2384,7 +2393,7 @@
       <c r="A14" s="26">
         <v>13</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="35" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -2397,36 +2406,36 @@
         <v>1</v>
       </c>
       <c r="F14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14" s="23">
-        <v>0</v>
-      </c>
-      <c r="P14" s="23">
+        <v>1</v>
+      </c>
+      <c r="P14" s="42">
         <v>0</v>
       </c>
       <c r="Q14" s="23">
@@ -2467,7 +2476,7 @@
       <c r="A15" s="26">
         <v>14</v>
       </c>
-      <c r="B15" s="35"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="13" t="s">
         <v>34</v>
       </c>
@@ -2478,36 +2487,36 @@
         <v>2</v>
       </c>
       <c r="F15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O15" s="23">
-        <v>0</v>
-      </c>
-      <c r="P15" s="23">
+        <v>2</v>
+      </c>
+      <c r="P15" s="42">
         <v>0</v>
       </c>
       <c r="Q15" s="23">
@@ -2548,7 +2557,7 @@
       <c r="A16" s="26">
         <v>15</v>
       </c>
-      <c r="B16" s="36"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="13" t="s">
         <v>35</v>
       </c>
@@ -2559,39 +2568,39 @@
         <v>4</v>
       </c>
       <c r="F16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P16" s="23">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="23">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="42">
         <v>0</v>
       </c>
       <c r="R16" s="23">
@@ -2629,7 +2638,7 @@
       <c r="A17" s="26">
         <v>16</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="40" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -2642,42 +2651,42 @@
         <v>1</v>
       </c>
       <c r="F17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="23">
-        <v>0</v>
-      </c>
-      <c r="R17" s="23">
+        <v>1</v>
+      </c>
+      <c r="R17" s="42">
         <v>0</v>
       </c>
       <c r="S17" s="23">
@@ -2712,7 +2721,7 @@
       <c r="A18" s="26">
         <v>17</v>
       </c>
-      <c r="B18" s="33"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="13" t="s">
         <v>38</v>
       </c>
@@ -2723,42 +2732,42 @@
         <v>2</v>
       </c>
       <c r="F18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q18" s="23">
-        <v>0</v>
-      </c>
-      <c r="R18" s="23">
+        <v>2</v>
+      </c>
+      <c r="R18" s="42">
         <v>0</v>
       </c>
       <c r="S18" s="23">
@@ -2793,7 +2802,7 @@
       <c r="A19" s="26">
         <v>18</v>
       </c>
-      <c r="B19" s="33"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="13" t="s">
         <v>39</v>
       </c>
@@ -2804,45 +2813,45 @@
         <v>2</v>
       </c>
       <c r="F19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R19" s="23">
-        <v>0</v>
-      </c>
-      <c r="S19" s="23">
+        <v>1</v>
+      </c>
+      <c r="S19" s="42">
         <v>0</v>
       </c>
       <c r="T19" s="23">
@@ -2874,7 +2883,7 @@
       <c r="A20" s="26">
         <v>19</v>
       </c>
-      <c r="B20" s="33"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="12" t="s">
         <v>40</v>
       </c>
@@ -2882,51 +2891,51 @@
         <v>6</v>
       </c>
       <c r="E20" s="27">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S20" s="23">
-        <v>0</v>
-      </c>
-      <c r="T20" s="23">
+        <v>2</v>
+      </c>
+      <c r="T20" s="42">
         <v>0</v>
       </c>
       <c r="U20" s="23">
@@ -2955,7 +2964,7 @@
       <c r="A21" s="26">
         <v>20</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="40" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -2967,49 +2976,49 @@
       <c r="E21" s="27">
         <v>1</v>
       </c>
-      <c r="F21" s="23">
-        <v>0</v>
-      </c>
-      <c r="G21" s="23">
-        <v>0</v>
-      </c>
-      <c r="H21" s="23">
-        <v>0</v>
-      </c>
-      <c r="I21" s="23">
-        <v>0</v>
-      </c>
-      <c r="J21" s="23">
-        <v>0</v>
-      </c>
-      <c r="K21" s="23">
-        <v>0</v>
-      </c>
-      <c r="L21" s="23">
-        <v>0</v>
-      </c>
-      <c r="M21" s="23">
-        <v>0</v>
-      </c>
-      <c r="N21" s="23">
-        <v>0</v>
-      </c>
-      <c r="O21" s="23">
-        <v>0</v>
-      </c>
-      <c r="P21" s="23">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="23">
-        <v>0</v>
-      </c>
-      <c r="R21" s="23">
-        <v>0</v>
-      </c>
-      <c r="S21" s="23">
-        <v>0</v>
-      </c>
-      <c r="T21" s="23">
+      <c r="F21" s="25">
+        <v>1</v>
+      </c>
+      <c r="G21" s="25">
+        <v>1</v>
+      </c>
+      <c r="H21" s="25">
+        <v>1</v>
+      </c>
+      <c r="I21" s="25">
+        <v>1</v>
+      </c>
+      <c r="J21" s="25">
+        <v>1</v>
+      </c>
+      <c r="K21" s="25">
+        <v>1</v>
+      </c>
+      <c r="L21" s="25">
+        <v>1</v>
+      </c>
+      <c r="M21" s="25">
+        <v>1</v>
+      </c>
+      <c r="N21" s="25">
+        <v>1</v>
+      </c>
+      <c r="O21" s="25">
+        <v>1</v>
+      </c>
+      <c r="P21" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="25">
+        <v>1</v>
+      </c>
+      <c r="R21" s="25">
+        <v>1</v>
+      </c>
+      <c r="S21" s="25">
+        <v>1</v>
+      </c>
+      <c r="T21" s="42">
         <v>0</v>
       </c>
       <c r="U21" s="23">
@@ -3038,7 +3047,7 @@
       <c r="A22" s="26">
         <v>21</v>
       </c>
-      <c r="B22" s="33"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="13" t="s">
         <v>43</v>
       </c>
@@ -3049,48 +3058,48 @@
         <v>1</v>
       </c>
       <c r="F22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S22" s="23">
-        <v>0</v>
-      </c>
-      <c r="T22" s="23">
+        <v>1</v>
+      </c>
+      <c r="T22" s="42">
         <v>0</v>
       </c>
       <c r="U22" s="23">
@@ -3119,7 +3128,7 @@
       <c r="A23" s="26">
         <v>22</v>
       </c>
-      <c r="B23" s="33"/>
+      <c r="B23" s="40"/>
       <c r="C23" s="13" t="s">
         <v>44</v>
       </c>
@@ -3130,51 +3139,51 @@
         <v>2</v>
       </c>
       <c r="F23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T23" s="23">
-        <v>0</v>
-      </c>
-      <c r="U23" s="23">
+        <v>2</v>
+      </c>
+      <c r="U23" s="42">
         <v>0</v>
       </c>
       <c r="V23" s="23">
@@ -3200,7 +3209,7 @@
       <c r="A24" s="26">
         <v>23</v>
       </c>
-      <c r="B24" s="33"/>
+      <c r="B24" s="40"/>
       <c r="C24" s="12" t="s">
         <v>45</v>
       </c>
@@ -3211,51 +3220,51 @@
         <v>2</v>
       </c>
       <c r="F24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T24" s="23">
-        <v>0</v>
-      </c>
-      <c r="U24" s="23">
+        <v>2</v>
+      </c>
+      <c r="U24" s="42">
         <v>0</v>
       </c>
       <c r="V24" s="23">
@@ -3281,7 +3290,7 @@
       <c r="A25" s="26">
         <v>24</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="40" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -3290,58 +3299,58 @@
       <c r="D25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="27" t="s">
-        <v>61</v>
+      <c r="E25" s="33">
+        <v>0.5</v>
       </c>
       <c r="F25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U25" s="23">
-        <v>0</v>
-      </c>
-      <c r="V25" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="V25" s="42">
         <v>0</v>
       </c>
       <c r="W25" s="23">
@@ -3364,7 +3373,7 @@
       <c r="A26" s="26">
         <v>25</v>
       </c>
-      <c r="B26" s="33"/>
+      <c r="B26" s="40"/>
       <c r="C26" s="13" t="s">
         <v>47</v>
       </c>
@@ -3375,54 +3384,54 @@
         <v>1</v>
       </c>
       <c r="F26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U26" s="23">
-        <v>0</v>
-      </c>
-      <c r="V26" s="23">
+        <v>1</v>
+      </c>
+      <c r="V26" s="42">
         <v>0</v>
       </c>
       <c r="W26" s="23">
@@ -3445,7 +3454,7 @@
       <c r="A27" s="26">
         <v>26</v>
       </c>
-      <c r="B27" s="33"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="13" t="s">
         <v>48</v>
       </c>
@@ -3456,54 +3465,54 @@
         <v>2</v>
       </c>
       <c r="F27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U27" s="23">
-        <v>0</v>
-      </c>
-      <c r="V27" s="23">
+        <v>2</v>
+      </c>
+      <c r="V27" s="42">
         <v>0</v>
       </c>
       <c r="W27" s="23">
@@ -3526,7 +3535,7 @@
       <c r="A28" s="26">
         <v>27</v>
       </c>
-      <c r="B28" s="33"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="12" t="s">
         <v>49</v>
       </c>
@@ -3537,57 +3546,57 @@
         <v>4</v>
       </c>
       <c r="F28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V28" s="23">
-        <v>0</v>
-      </c>
-      <c r="W28" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="W28" s="42">
         <v>0</v>
       </c>
       <c r="X28" s="23">
@@ -3616,29 +3625,69 @@
       <c r="D29" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="23"/>
-      <c r="V29" s="23"/>
-      <c r="W29" s="23"/>
-      <c r="X29" s="23"/>
-      <c r="Y29" s="23"/>
+      <c r="E29" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="F29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="H29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="I29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="J29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="K29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="L29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="N29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="O29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="R29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="S29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="T29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="U29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="V29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="W29" s="42">
+        <v>0</v>
+      </c>
+      <c r="X29" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="23">
+        <v>0</v>
+      </c>
       <c r="Z29" s="7"/>
       <c r="AA29" s="7"/>
       <c r="AB29" s="7"/>
@@ -3660,26 +3709,66 @@
       <c r="E30" s="30">
         <v>1</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="23"/>
-      <c r="Q30" s="23"/>
-      <c r="R30" s="23"/>
-      <c r="S30" s="23"/>
-      <c r="T30" s="23"/>
-      <c r="U30" s="23"/>
-      <c r="V30" s="23"/>
-      <c r="W30" s="23"/>
-      <c r="X30" s="23"/>
-      <c r="Y30" s="23"/>
+      <c r="F30" s="23">
+        <v>1</v>
+      </c>
+      <c r="G30" s="23">
+        <v>1</v>
+      </c>
+      <c r="H30" s="23">
+        <v>1</v>
+      </c>
+      <c r="I30" s="23">
+        <v>1</v>
+      </c>
+      <c r="J30" s="23">
+        <v>1</v>
+      </c>
+      <c r="K30" s="23">
+        <v>1</v>
+      </c>
+      <c r="L30" s="23">
+        <v>1</v>
+      </c>
+      <c r="M30" s="23">
+        <v>1</v>
+      </c>
+      <c r="N30" s="23">
+        <v>1</v>
+      </c>
+      <c r="O30" s="23">
+        <v>1</v>
+      </c>
+      <c r="P30" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="23">
+        <v>1</v>
+      </c>
+      <c r="R30" s="23">
+        <v>1</v>
+      </c>
+      <c r="S30" s="23">
+        <v>1</v>
+      </c>
+      <c r="T30" s="23">
+        <v>1</v>
+      </c>
+      <c r="U30" s="23">
+        <v>1</v>
+      </c>
+      <c r="V30" s="23">
+        <v>1</v>
+      </c>
+      <c r="W30" s="23">
+        <v>1</v>
+      </c>
+      <c r="X30" s="42">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="23">
+        <v>0</v>
+      </c>
       <c r="Z30" s="7"/>
       <c r="AA30" s="7"/>
       <c r="AB30" s="7"/>
@@ -3691,7 +3780,7 @@
       <c r="A31" s="26">
         <v>30</v>
       </c>
-      <c r="B31" s="38"/>
+      <c r="B31" s="36"/>
       <c r="C31" s="13" t="s">
         <v>59</v>
       </c>
@@ -3701,26 +3790,66 @@
       <c r="E31" s="30">
         <v>4</v>
       </c>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="23"/>
-      <c r="Q31" s="23"/>
-      <c r="R31" s="23"/>
-      <c r="S31" s="23"/>
-      <c r="T31" s="23"/>
-      <c r="U31" s="23"/>
-      <c r="V31" s="23"/>
-      <c r="W31" s="23"/>
-      <c r="X31" s="23"/>
-      <c r="Y31" s="23"/>
+      <c r="F31" s="23">
+        <v>4</v>
+      </c>
+      <c r="G31" s="23">
+        <v>4</v>
+      </c>
+      <c r="H31" s="23">
+        <v>4</v>
+      </c>
+      <c r="I31" s="23">
+        <v>4</v>
+      </c>
+      <c r="J31" s="23">
+        <v>4</v>
+      </c>
+      <c r="K31" s="23">
+        <v>4</v>
+      </c>
+      <c r="L31" s="23">
+        <v>4</v>
+      </c>
+      <c r="M31" s="23">
+        <v>4</v>
+      </c>
+      <c r="N31" s="23">
+        <v>4</v>
+      </c>
+      <c r="O31" s="23">
+        <v>4</v>
+      </c>
+      <c r="P31" s="23">
+        <v>4</v>
+      </c>
+      <c r="Q31" s="23">
+        <v>4</v>
+      </c>
+      <c r="R31" s="23">
+        <v>4</v>
+      </c>
+      <c r="S31" s="23">
+        <v>4</v>
+      </c>
+      <c r="T31" s="23">
+        <v>4</v>
+      </c>
+      <c r="U31" s="23">
+        <v>4</v>
+      </c>
+      <c r="V31" s="23">
+        <v>4</v>
+      </c>
+      <c r="W31" s="23">
+        <v>4</v>
+      </c>
+      <c r="X31" s="23">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="42">
+        <v>0</v>
+      </c>
       <c r="Z31" s="7"/>
       <c r="AA31" s="7"/>
       <c r="AB31" s="7"/>
@@ -3732,74 +3861,74 @@
       <c r="A32" s="26">
         <v>31</v>
       </c>
-      <c r="B32" s="34"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="27" t="s">
-        <v>61</v>
+      <c r="E32" s="33">
+        <v>0.5</v>
       </c>
       <c r="F32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X32" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y32" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Y32" s="42">
         <v>0</v>
       </c>
       <c r="Z32" s="7"/>
@@ -3813,74 +3942,74 @@
       <c r="A33" s="26">
         <v>32</v>
       </c>
-      <c r="B33" s="35"/>
+      <c r="B33" s="38"/>
       <c r="C33" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="27" t="s">
-        <v>61</v>
+      <c r="E33" s="33">
+        <v>0.5</v>
       </c>
       <c r="F33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X33" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y33" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Y33" s="42">
         <v>0</v>
       </c>
       <c r="Z33" s="7"/>
@@ -3894,74 +4023,74 @@
       <c r="A34" s="26">
         <v>33</v>
       </c>
-      <c r="B34" s="35"/>
+      <c r="B34" s="38"/>
       <c r="C34" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E34" s="27" t="s">
-        <v>61</v>
+      <c r="E34" s="33">
+        <v>0.5</v>
       </c>
       <c r="F34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X34" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y34" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Y34" s="42">
         <v>0</v>
       </c>
       <c r="Z34" s="7"/>
@@ -3975,74 +4104,74 @@
       <c r="A35" s="26">
         <v>34</v>
       </c>
-      <c r="B35" s="35"/>
+      <c r="B35" s="38"/>
       <c r="C35" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="27" t="s">
-        <v>61</v>
+      <c r="E35" s="33">
+        <v>0.5</v>
       </c>
       <c r="F35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X35" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y35" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Y35" s="42">
         <v>0</v>
       </c>
       <c r="Z35" s="7"/>
@@ -4056,74 +4185,74 @@
       <c r="A36" s="26">
         <v>35</v>
       </c>
-      <c r="B36" s="35"/>
+      <c r="B36" s="38"/>
       <c r="C36" s="12" t="s">
         <v>54</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="27" t="s">
-        <v>61</v>
+      <c r="E36" s="33">
+        <v>0.5</v>
       </c>
       <c r="F36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X36" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Y36" s="42">
         <v>0</v>
       </c>
       <c r="Z36" s="7"/>
@@ -4137,34 +4266,76 @@
       <c r="A37" s="26">
         <v>36</v>
       </c>
-      <c r="B37" s="36"/>
+      <c r="B37" s="39"/>
       <c r="C37" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="23"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="23"/>
-      <c r="N37" s="23"/>
-      <c r="O37" s="23"/>
-      <c r="P37" s="23"/>
-      <c r="Q37" s="23"/>
-      <c r="R37" s="23"/>
-      <c r="S37" s="23"/>
-      <c r="T37" s="23"/>
-      <c r="U37" s="23"/>
-      <c r="V37" s="23"/>
-      <c r="W37" s="23"/>
-      <c r="X37" s="23"/>
-      <c r="Y37" s="23"/>
+      <c r="D37" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="F37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="G37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="H37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="I37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="J37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="K37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="L37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="N37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="O37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="P37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Q37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="R37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="S37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="T37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="U37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="V37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="W37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="X37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="Y37" s="42">
+        <v>0</v>
+      </c>
       <c r="Z37" s="7"/>
       <c r="AA37" s="7"/>
       <c r="AB37" s="7"/>
@@ -4509,79 +4680,79 @@
       </c>
       <c r="F42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="G42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="H42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="I42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="J42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="L42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="M42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="N42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="O42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="P42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="Q42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="R42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="S42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="T42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="U42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="V42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="W42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X42" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y42" s="1">
         <f t="shared" si="0"/>
@@ -4596,16 +4767,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="B29:B31"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="B29:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4616,8 +4787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4739,8 +4910,8 @@
       <c r="D2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="27">
-        <v>0</v>
+      <c r="E2" s="34">
+        <v>5</v>
       </c>
       <c r="F2" s="32"/>
       <c r="G2" s="23">
@@ -4808,7 +4979,7 @@
       <c r="A3" s="26">
         <v>2</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="35" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -4817,8 +4988,8 @@
       <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="27">
-        <v>0</v>
+      <c r="E3" s="34">
+        <v>4</v>
       </c>
       <c r="F3" s="32"/>
       <c r="G3" s="23">
@@ -4886,15 +5057,15 @@
       <c r="A4" s="26">
         <v>3</v>
       </c>
-      <c r="B4" s="38"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="27">
-        <v>0</v>
+      <c r="E4" s="34">
+        <v>6</v>
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="23">
@@ -4962,7 +5133,7 @@
       <c r="A5" s="26">
         <v>4</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="35" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="29" t="s">
@@ -4971,8 +5142,8 @@
       <c r="D5" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="27">
-        <v>0</v>
+      <c r="E5" s="34">
+        <v>1</v>
       </c>
       <c r="F5" s="32"/>
       <c r="G5" s="23">
@@ -5040,15 +5211,15 @@
       <c r="A6" s="26">
         <v>5</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="27">
-        <v>0</v>
+      <c r="E6" s="34">
+        <v>8</v>
       </c>
       <c r="F6" s="32"/>
       <c r="G6" s="23">
@@ -5116,7 +5287,7 @@
       <c r="A7" s="26">
         <v>6</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="35" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -5125,8 +5296,8 @@
       <c r="D7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="27">
-        <v>0</v>
+      <c r="E7" s="34">
+        <v>0.5</v>
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="23">
@@ -5201,8 +5372,8 @@
       <c r="D8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="27">
-        <v>0</v>
+      <c r="E8" s="34">
+        <v>1</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="23">
@@ -5270,15 +5441,15 @@
       <c r="A9" s="26">
         <v>8</v>
       </c>
-      <c r="B9" s="38"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="27">
-        <v>0</v>
+      <c r="E9" s="34">
+        <v>1</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="23">
@@ -5346,7 +5517,7 @@
       <c r="A10" s="26">
         <v>9</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="35" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -5355,8 +5526,8 @@
       <c r="D10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="27">
-        <v>0</v>
+      <c r="E10" s="34">
+        <v>0.5</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="23">
@@ -5431,8 +5602,8 @@
       <c r="D11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="27">
-        <v>0</v>
+      <c r="E11" s="34">
+        <v>4</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="23">
@@ -5507,8 +5678,8 @@
       <c r="D12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="27">
-        <v>0</v>
+      <c r="E12" s="34">
+        <v>2</v>
       </c>
       <c r="F12" s="32"/>
       <c r="G12" s="23">
@@ -5576,15 +5747,15 @@
       <c r="A13" s="26">
         <v>12</v>
       </c>
-      <c r="B13" s="38"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="17" t="s">
         <v>31</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="27">
-        <v>0</v>
+      <c r="E13" s="34">
+        <v>4</v>
       </c>
       <c r="F13" s="32"/>
       <c r="G13" s="23">
@@ -5652,7 +5823,7 @@
       <c r="A14" s="26">
         <v>13</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="35" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -5661,8 +5832,8 @@
       <c r="D14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="27">
-        <v>0</v>
+      <c r="E14" s="34">
+        <v>1</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="23">
@@ -5730,15 +5901,15 @@
       <c r="A15" s="26">
         <v>14</v>
       </c>
-      <c r="B15" s="35"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="13" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="27">
-        <v>0</v>
+      <c r="E15" s="34">
+        <v>2</v>
       </c>
       <c r="F15" s="32"/>
       <c r="G15" s="23">
@@ -5806,15 +5977,15 @@
       <c r="A16" s="26">
         <v>15</v>
       </c>
-      <c r="B16" s="36"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="13" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="27">
-        <v>0</v>
+      <c r="E16" s="34">
+        <v>4</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="23">
@@ -5882,7 +6053,7 @@
       <c r="A17" s="26">
         <v>16</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="40" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -5891,8 +6062,8 @@
       <c r="D17" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="27">
-        <v>0</v>
+      <c r="E17" s="34">
+        <v>1</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="23">
@@ -5960,15 +6131,15 @@
       <c r="A18" s="26">
         <v>17</v>
       </c>
-      <c r="B18" s="33"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="13" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="27">
-        <v>0</v>
+      <c r="E18" s="34">
+        <v>2</v>
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="23">
@@ -6036,15 +6207,15 @@
       <c r="A19" s="26">
         <v>18</v>
       </c>
-      <c r="B19" s="33"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="13" t="s">
         <v>39</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="27">
-        <v>0</v>
+      <c r="E19" s="34">
+        <v>2</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="23">
@@ -6112,15 +6283,15 @@
       <c r="A20" s="26">
         <v>19</v>
       </c>
-      <c r="B20" s="33"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="27">
-        <v>0</v>
+      <c r="E20" s="34">
+        <v>5</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="23">
@@ -6188,7 +6359,7 @@
       <c r="A21" s="26">
         <v>20</v>
       </c>
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="40" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -6197,8 +6368,8 @@
       <c r="D21" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="27">
-        <v>0</v>
+      <c r="E21" s="34">
+        <v>1</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="23">
@@ -6266,15 +6437,15 @@
       <c r="A22" s="26">
         <v>21</v>
       </c>
-      <c r="B22" s="33"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="13" t="s">
         <v>43</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="27">
-        <v>0</v>
+      <c r="E22" s="34">
+        <v>1</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="23">
@@ -6342,15 +6513,15 @@
       <c r="A23" s="26">
         <v>22</v>
       </c>
-      <c r="B23" s="33"/>
+      <c r="B23" s="40"/>
       <c r="C23" s="13" t="s">
         <v>44</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="27">
-        <v>0</v>
+      <c r="E23" s="34">
+        <v>2</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="23">
@@ -6418,15 +6589,15 @@
       <c r="A24" s="26">
         <v>23</v>
       </c>
-      <c r="B24" s="33"/>
+      <c r="B24" s="40"/>
       <c r="C24" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="27">
-        <v>0</v>
+      <c r="E24" s="34">
+        <v>2</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="23">
@@ -6494,7 +6665,7 @@
       <c r="A25" s="26">
         <v>24</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="40" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -6503,8 +6674,8 @@
       <c r="D25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="27">
-        <v>0</v>
+      <c r="E25" s="34">
+        <v>0.5</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="23">
@@ -6572,15 +6743,15 @@
       <c r="A26" s="26">
         <v>25</v>
       </c>
-      <c r="B26" s="33"/>
+      <c r="B26" s="40"/>
       <c r="C26" s="13" t="s">
         <v>47</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="27">
-        <v>0</v>
+      <c r="E26" s="34">
+        <v>1</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="23">
@@ -6648,15 +6819,15 @@
       <c r="A27" s="26">
         <v>26</v>
       </c>
-      <c r="B27" s="33"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="13" t="s">
         <v>48</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="27">
-        <v>0</v>
+      <c r="E27" s="34">
+        <v>2</v>
       </c>
       <c r="F27" s="32"/>
       <c r="G27" s="23">
@@ -6724,15 +6895,15 @@
       <c r="A28" s="26">
         <v>27</v>
       </c>
-      <c r="B28" s="33"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="12" t="s">
         <v>49</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="27">
-        <v>0</v>
+      <c r="E28" s="34">
+        <v>4</v>
       </c>
       <c r="F28" s="32"/>
       <c r="G28" s="23">
@@ -6809,30 +6980,70 @@
       <c r="D29" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E29" s="30">
-        <v>0</v>
+      <c r="E29" s="34">
+        <v>0.5</v>
       </c>
       <c r="F29" s="32"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-      <c r="R29" s="23"/>
-      <c r="S29" s="23"/>
-      <c r="T29" s="23"/>
-      <c r="U29" s="23"/>
-      <c r="V29" s="23"/>
-      <c r="W29" s="23"/>
-      <c r="X29" s="23"/>
-      <c r="Y29" s="23"/>
-      <c r="Z29" s="23"/>
+      <c r="G29" s="23">
+        <v>0</v>
+      </c>
+      <c r="H29" s="23">
+        <v>0</v>
+      </c>
+      <c r="I29" s="23">
+        <v>0</v>
+      </c>
+      <c r="J29" s="23">
+        <v>0</v>
+      </c>
+      <c r="K29" s="23">
+        <v>0</v>
+      </c>
+      <c r="L29" s="23">
+        <v>0</v>
+      </c>
+      <c r="M29" s="23">
+        <v>0</v>
+      </c>
+      <c r="N29" s="23">
+        <v>0</v>
+      </c>
+      <c r="O29" s="23">
+        <v>0</v>
+      </c>
+      <c r="P29" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="23">
+        <v>0</v>
+      </c>
+      <c r="R29" s="23">
+        <v>0</v>
+      </c>
+      <c r="S29" s="23">
+        <v>0</v>
+      </c>
+      <c r="T29" s="23">
+        <v>0</v>
+      </c>
+      <c r="U29" s="23">
+        <v>0</v>
+      </c>
+      <c r="V29" s="23">
+        <v>0</v>
+      </c>
+      <c r="W29" s="23">
+        <v>0</v>
+      </c>
+      <c r="X29" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="23">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:26" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="26">
@@ -6845,80 +7056,160 @@
       <c r="D30" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="30">
-        <v>0</v>
+      <c r="E30" s="34">
+        <v>1</v>
       </c>
       <c r="F30" s="32"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="23"/>
-      <c r="Q30" s="23"/>
-      <c r="R30" s="23"/>
-      <c r="S30" s="23"/>
-      <c r="T30" s="23"/>
-      <c r="U30" s="23"/>
-      <c r="V30" s="23"/>
-      <c r="W30" s="23"/>
-      <c r="X30" s="23"/>
-      <c r="Y30" s="23"/>
-      <c r="Z30" s="23"/>
+      <c r="G30" s="23">
+        <v>0</v>
+      </c>
+      <c r="H30" s="23">
+        <v>0</v>
+      </c>
+      <c r="I30" s="23">
+        <v>0</v>
+      </c>
+      <c r="J30" s="23">
+        <v>0</v>
+      </c>
+      <c r="K30" s="23">
+        <v>0</v>
+      </c>
+      <c r="L30" s="23">
+        <v>0</v>
+      </c>
+      <c r="M30" s="23">
+        <v>0</v>
+      </c>
+      <c r="N30" s="23">
+        <v>0</v>
+      </c>
+      <c r="O30" s="23">
+        <v>0</v>
+      </c>
+      <c r="P30" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="23">
+        <v>0</v>
+      </c>
+      <c r="R30" s="23">
+        <v>0</v>
+      </c>
+      <c r="S30" s="23">
+        <v>0</v>
+      </c>
+      <c r="T30" s="23">
+        <v>0</v>
+      </c>
+      <c r="U30" s="23">
+        <v>0</v>
+      </c>
+      <c r="V30" s="23">
+        <v>0</v>
+      </c>
+      <c r="W30" s="23">
+        <v>0</v>
+      </c>
+      <c r="X30" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="23">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:26" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="26">
         <v>30</v>
       </c>
-      <c r="B31" s="38"/>
+      <c r="B31" s="36"/>
       <c r="C31" s="13" t="s">
         <v>59</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="30">
-        <v>0</v>
+      <c r="E31" s="34">
+        <v>4</v>
       </c>
       <c r="F31" s="32"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="23"/>
-      <c r="Q31" s="23"/>
-      <c r="R31" s="23"/>
-      <c r="S31" s="23"/>
-      <c r="T31" s="23"/>
-      <c r="U31" s="23"/>
-      <c r="V31" s="23"/>
-      <c r="W31" s="23"/>
-      <c r="X31" s="23"/>
-      <c r="Y31" s="23"/>
-      <c r="Z31" s="23"/>
+      <c r="G31" s="23">
+        <v>0</v>
+      </c>
+      <c r="H31" s="23">
+        <v>0</v>
+      </c>
+      <c r="I31" s="23">
+        <v>0</v>
+      </c>
+      <c r="J31" s="23">
+        <v>0</v>
+      </c>
+      <c r="K31" s="23">
+        <v>0</v>
+      </c>
+      <c r="L31" s="23">
+        <v>0</v>
+      </c>
+      <c r="M31" s="23">
+        <v>0</v>
+      </c>
+      <c r="N31" s="23">
+        <v>0</v>
+      </c>
+      <c r="O31" s="23">
+        <v>0</v>
+      </c>
+      <c r="P31" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="23">
+        <v>0</v>
+      </c>
+      <c r="R31" s="23">
+        <v>0</v>
+      </c>
+      <c r="S31" s="23">
+        <v>0</v>
+      </c>
+      <c r="T31" s="23">
+        <v>0</v>
+      </c>
+      <c r="U31" s="23">
+        <v>0</v>
+      </c>
+      <c r="V31" s="23">
+        <v>0</v>
+      </c>
+      <c r="W31" s="23">
+        <v>0</v>
+      </c>
+      <c r="X31" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="23">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26">
         <v>31</v>
       </c>
-      <c r="B32" s="34"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="27">
-        <v>0</v>
+      <c r="E32" s="34">
+        <v>0.5</v>
       </c>
       <c r="F32" s="32"/>
       <c r="G32" s="23">
@@ -6986,15 +7277,15 @@
       <c r="A33" s="26">
         <v>32</v>
       </c>
-      <c r="B33" s="35"/>
+      <c r="B33" s="38"/>
       <c r="C33" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="27">
-        <v>0</v>
+      <c r="E33" s="34">
+        <v>0.5</v>
       </c>
       <c r="F33" s="32"/>
       <c r="G33" s="23">
@@ -7062,15 +7353,15 @@
       <c r="A34" s="26">
         <v>33</v>
       </c>
-      <c r="B34" s="35"/>
+      <c r="B34" s="38"/>
       <c r="C34" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E34" s="27">
-        <v>0</v>
+      <c r="E34" s="34">
+        <v>0.5</v>
       </c>
       <c r="F34" s="32"/>
       <c r="G34" s="23">
@@ -7138,15 +7429,15 @@
       <c r="A35" s="26">
         <v>34</v>
       </c>
-      <c r="B35" s="35"/>
+      <c r="B35" s="38"/>
       <c r="C35" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="27">
-        <v>0</v>
+      <c r="E35" s="34">
+        <v>0.5</v>
       </c>
       <c r="F35" s="32"/>
       <c r="G35" s="23">
@@ -7214,15 +7505,15 @@
       <c r="A36" s="26">
         <v>35</v>
       </c>
-      <c r="B36" s="35"/>
+      <c r="B36" s="38"/>
       <c r="C36" s="12" t="s">
         <v>54</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="27">
-        <v>0</v>
+      <c r="E36" s="34">
+        <v>0.5</v>
       </c>
       <c r="F36" s="32"/>
       <c r="G36" s="23">
@@ -7290,33 +7581,77 @@
       <c r="A37" s="26">
         <v>36</v>
       </c>
-      <c r="B37" s="36"/>
+      <c r="B37" s="39"/>
       <c r="C37" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="30"/>
+      <c r="D37" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="34">
+        <v>0.5</v>
+      </c>
       <c r="F37" s="32"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="23"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="23"/>
-      <c r="N37" s="23"/>
-      <c r="O37" s="23"/>
-      <c r="P37" s="23"/>
-      <c r="Q37" s="23"/>
-      <c r="R37" s="23"/>
-      <c r="S37" s="23"/>
-      <c r="T37" s="23"/>
-      <c r="U37" s="23"/>
-      <c r="V37" s="23"/>
-      <c r="W37" s="23"/>
-      <c r="X37" s="23"/>
-      <c r="Y37" s="23"/>
-      <c r="Z37" s="23"/>
+      <c r="G37" s="23">
+        <v>0</v>
+      </c>
+      <c r="H37" s="23">
+        <v>0</v>
+      </c>
+      <c r="I37" s="23">
+        <v>0</v>
+      </c>
+      <c r="J37" s="23">
+        <v>0</v>
+      </c>
+      <c r="K37" s="23">
+        <v>0</v>
+      </c>
+      <c r="L37" s="23">
+        <v>0</v>
+      </c>
+      <c r="M37" s="23">
+        <v>0</v>
+      </c>
+      <c r="N37" s="23">
+        <v>0</v>
+      </c>
+      <c r="O37" s="23">
+        <v>0</v>
+      </c>
+      <c r="P37" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="23">
+        <v>0</v>
+      </c>
+      <c r="R37" s="23">
+        <v>0</v>
+      </c>
+      <c r="S37" s="23">
+        <v>0</v>
+      </c>
+      <c r="T37" s="23">
+        <v>0</v>
+      </c>
+      <c r="U37" s="23">
+        <v>0</v>
+      </c>
+      <c r="V37" s="23">
+        <v>0</v>
+      </c>
+      <c r="W37" s="23">
+        <v>0</v>
+      </c>
+      <c r="X37" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="23">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="23">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26">
@@ -7699,7 +8034,7 @@
       <c r="D43" s="22"/>
       <c r="E43" s="2">
         <f>SUM(E2:E41)</f>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="F43" s="27" t="s">
         <v>4</v>
@@ -7787,16 +8122,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B37"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B32:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update progress of print 2
</commit_message>
<xml_diff>
--- a/7.Print-Backlog/Sprint-2.xlsx
+++ b/7.Print-Backlog/Sprint-2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimate" sheetId="1" r:id="rId1"/>
@@ -522,14 +522,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -537,13 +537,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -832,22 +832,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -906,11 +906,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="207074816"/>
-        <c:axId val="207076352"/>
+        <c:axId val="189969920"/>
+        <c:axId val="189971456"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="207074816"/>
+        <c:axId val="189969920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,14 +920,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="207076352"/>
+        <c:crossAx val="189971456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="207076352"/>
+        <c:axId val="189971456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,7 +938,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="207074816"/>
+        <c:crossAx val="189969920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1293,7 +1293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="C36" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1429,7 +1429,7 @@
       <c r="G2" s="23">
         <v>1</v>
       </c>
-      <c r="H2" s="42">
+      <c r="H2" s="35">
         <v>0</v>
       </c>
       <c r="I2" s="23">
@@ -1494,7 +1494,7 @@
       <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="42" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -1515,7 +1515,7 @@
       <c r="H3" s="23">
         <v>1</v>
       </c>
-      <c r="I3" s="42">
+      <c r="I3" s="35">
         <v>0</v>
       </c>
       <c r="J3" s="23">
@@ -1577,7 +1577,7 @@
       <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="36"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="16" t="s">
         <v>20</v>
       </c>
@@ -1599,7 +1599,7 @@
       <c r="I4" s="23">
         <v>3</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="35">
         <v>0</v>
       </c>
       <c r="K4" s="23">
@@ -1658,7 +1658,7 @@
       <c r="A5" s="26">
         <v>4</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="42" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="29" t="s">
@@ -1682,10 +1682,10 @@
       <c r="I5" s="23">
         <v>1</v>
       </c>
-      <c r="J5" s="42">
-        <v>0</v>
-      </c>
-      <c r="K5" s="42">
+      <c r="J5" s="35">
+        <v>0</v>
+      </c>
+      <c r="K5" s="35">
         <v>0</v>
       </c>
       <c r="L5" s="23">
@@ -1741,7 +1741,7 @@
       <c r="A6" s="26">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="13" t="s">
         <v>14</v>
       </c>
@@ -1769,7 +1769,7 @@
       <c r="K6" s="23">
         <v>4</v>
       </c>
-      <c r="L6" s="42">
+      <c r="L6" s="35">
         <v>0</v>
       </c>
       <c r="M6" s="23">
@@ -1822,7 +1822,7 @@
       <c r="A7" s="26">
         <v>6</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="42" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -1855,7 +1855,7 @@
       <c r="L7" s="23">
         <v>0.5</v>
       </c>
-      <c r="M7" s="42">
+      <c r="M7" s="35">
         <v>0</v>
       </c>
       <c r="N7" s="23">
@@ -1905,7 +1905,7 @@
       <c r="A8" s="26">
         <v>7</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="13" t="s">
         <v>22</v>
       </c>
@@ -1936,7 +1936,7 @@
       <c r="L8" s="23">
         <v>1</v>
       </c>
-      <c r="M8" s="42">
+      <c r="M8" s="35">
         <v>0</v>
       </c>
       <c r="N8" s="23">
@@ -1986,7 +1986,7 @@
       <c r="A9" s="26">
         <v>8</v>
       </c>
-      <c r="B9" s="36"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="13" t="s">
         <v>15</v>
       </c>
@@ -2017,7 +2017,7 @@
       <c r="L9" s="23">
         <v>1</v>
       </c>
-      <c r="M9" s="42">
+      <c r="M9" s="35">
         <v>0</v>
       </c>
       <c r="N9" s="23">
@@ -2067,7 +2067,7 @@
       <c r="A10" s="26">
         <v>9</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="42" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -2100,7 +2100,7 @@
       <c r="L10" s="23">
         <v>0.5</v>
       </c>
-      <c r="M10" s="42">
+      <c r="M10" s="35">
         <v>0</v>
       </c>
       <c r="N10" s="23">
@@ -2150,7 +2150,7 @@
       <c r="A11" s="26">
         <v>10</v>
       </c>
-      <c r="B11" s="37"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="13" t="s">
         <v>29</v>
       </c>
@@ -2184,7 +2184,7 @@
       <c r="M11" s="23">
         <v>3</v>
       </c>
-      <c r="N11" s="42">
+      <c r="N11" s="35">
         <v>0</v>
       </c>
       <c r="O11" s="23">
@@ -2231,7 +2231,7 @@
       <c r="A12" s="26">
         <v>11</v>
       </c>
-      <c r="B12" s="37"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="17" t="s">
         <v>30</v>
       </c>
@@ -2268,7 +2268,7 @@
       <c r="N12" s="23">
         <v>1</v>
       </c>
-      <c r="O12" s="42">
+      <c r="O12" s="35">
         <v>0</v>
       </c>
       <c r="P12" s="23">
@@ -2312,7 +2312,7 @@
       <c r="A13" s="26">
         <v>12</v>
       </c>
-      <c r="B13" s="36"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="17" t="s">
         <v>31</v>
       </c>
@@ -2352,7 +2352,7 @@
       <c r="O13" s="23">
         <v>1</v>
       </c>
-      <c r="P13" s="42">
+      <c r="P13" s="35">
         <v>0</v>
       </c>
       <c r="Q13" s="23">
@@ -2393,7 +2393,7 @@
       <c r="A14" s="26">
         <v>13</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="42" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -2435,7 +2435,7 @@
       <c r="O14" s="23">
         <v>1</v>
       </c>
-      <c r="P14" s="42">
+      <c r="P14" s="35">
         <v>0</v>
       </c>
       <c r="Q14" s="23">
@@ -2516,7 +2516,7 @@
       <c r="O15" s="23">
         <v>2</v>
       </c>
-      <c r="P15" s="42">
+      <c r="P15" s="35">
         <v>0</v>
       </c>
       <c r="Q15" s="23">
@@ -2600,7 +2600,7 @@
       <c r="P16" s="23">
         <v>4</v>
       </c>
-      <c r="Q16" s="42">
+      <c r="Q16" s="35">
         <v>0</v>
       </c>
       <c r="R16" s="23">
@@ -2638,7 +2638,7 @@
       <c r="A17" s="26">
         <v>16</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="36" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -2686,7 +2686,7 @@
       <c r="Q17" s="23">
         <v>1</v>
       </c>
-      <c r="R17" s="42">
+      <c r="R17" s="35">
         <v>0</v>
       </c>
       <c r="S17" s="23">
@@ -2721,7 +2721,7 @@
       <c r="A18" s="26">
         <v>17</v>
       </c>
-      <c r="B18" s="40"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="13" t="s">
         <v>38</v>
       </c>
@@ -2767,7 +2767,7 @@
       <c r="Q18" s="23">
         <v>2</v>
       </c>
-      <c r="R18" s="42">
+      <c r="R18" s="35">
         <v>0</v>
       </c>
       <c r="S18" s="23">
@@ -2802,7 +2802,7 @@
       <c r="A19" s="26">
         <v>18</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="13" t="s">
         <v>39</v>
       </c>
@@ -2851,7 +2851,7 @@
       <c r="R19" s="23">
         <v>1</v>
       </c>
-      <c r="S19" s="42">
+      <c r="S19" s="35">
         <v>0</v>
       </c>
       <c r="T19" s="23">
@@ -2883,7 +2883,7 @@
       <c r="A20" s="26">
         <v>19</v>
       </c>
-      <c r="B20" s="40"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="12" t="s">
         <v>40</v>
       </c>
@@ -2935,7 +2935,7 @@
       <c r="S20" s="23">
         <v>2</v>
       </c>
-      <c r="T20" s="42">
+      <c r="T20" s="35">
         <v>0</v>
       </c>
       <c r="U20" s="23">
@@ -2964,7 +2964,7 @@
       <c r="A21" s="26">
         <v>20</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="36" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -3018,7 +3018,7 @@
       <c r="S21" s="25">
         <v>1</v>
       </c>
-      <c r="T21" s="42">
+      <c r="T21" s="35">
         <v>0</v>
       </c>
       <c r="U21" s="23">
@@ -3047,7 +3047,7 @@
       <c r="A22" s="26">
         <v>21</v>
       </c>
-      <c r="B22" s="40"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="13" t="s">
         <v>43</v>
       </c>
@@ -3099,7 +3099,7 @@
       <c r="S22" s="23">
         <v>1</v>
       </c>
-      <c r="T22" s="42">
+      <c r="T22" s="35">
         <v>0</v>
       </c>
       <c r="U22" s="23">
@@ -3128,7 +3128,7 @@
       <c r="A23" s="26">
         <v>22</v>
       </c>
-      <c r="B23" s="40"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="13" t="s">
         <v>44</v>
       </c>
@@ -3183,7 +3183,7 @@
       <c r="T23" s="23">
         <v>2</v>
       </c>
-      <c r="U23" s="42">
+      <c r="U23" s="35">
         <v>0</v>
       </c>
       <c r="V23" s="23">
@@ -3209,7 +3209,7 @@
       <c r="A24" s="26">
         <v>23</v>
       </c>
-      <c r="B24" s="40"/>
+      <c r="B24" s="36"/>
       <c r="C24" s="12" t="s">
         <v>45</v>
       </c>
@@ -3264,7 +3264,7 @@
       <c r="T24" s="23">
         <v>2</v>
       </c>
-      <c r="U24" s="42">
+      <c r="U24" s="35">
         <v>0</v>
       </c>
       <c r="V24" s="23">
@@ -3290,7 +3290,7 @@
       <c r="A25" s="26">
         <v>24</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="36" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -3350,7 +3350,7 @@
       <c r="U25" s="23">
         <v>0.5</v>
       </c>
-      <c r="V25" s="42">
+      <c r="V25" s="35">
         <v>0</v>
       </c>
       <c r="W25" s="23">
@@ -3373,7 +3373,7 @@
       <c r="A26" s="26">
         <v>25</v>
       </c>
-      <c r="B26" s="40"/>
+      <c r="B26" s="36"/>
       <c r="C26" s="13" t="s">
         <v>47</v>
       </c>
@@ -3431,7 +3431,7 @@
       <c r="U26" s="23">
         <v>1</v>
       </c>
-      <c r="V26" s="42">
+      <c r="V26" s="35">
         <v>0</v>
       </c>
       <c r="W26" s="23">
@@ -3454,7 +3454,7 @@
       <c r="A27" s="26">
         <v>26</v>
       </c>
-      <c r="B27" s="40"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="13" t="s">
         <v>48</v>
       </c>
@@ -3512,7 +3512,7 @@
       <c r="U27" s="23">
         <v>2</v>
       </c>
-      <c r="V27" s="42">
+      <c r="V27" s="35">
         <v>0</v>
       </c>
       <c r="W27" s="23">
@@ -3535,7 +3535,7 @@
       <c r="A28" s="26">
         <v>27</v>
       </c>
-      <c r="B28" s="40"/>
+      <c r="B28" s="36"/>
       <c r="C28" s="12" t="s">
         <v>49</v>
       </c>
@@ -3596,7 +3596,7 @@
       <c r="V28" s="23">
         <v>3.5</v>
       </c>
-      <c r="W28" s="42">
+      <c r="W28" s="35">
         <v>0</v>
       </c>
       <c r="X28" s="23">
@@ -3616,7 +3616,7 @@
       <c r="A29" s="26">
         <v>28</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="40" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="13" t="s">
@@ -3679,7 +3679,7 @@
       <c r="V29" s="23">
         <v>0.5</v>
       </c>
-      <c r="W29" s="42">
+      <c r="W29" s="35">
         <v>0</v>
       </c>
       <c r="X29" s="23">
@@ -3699,7 +3699,7 @@
       <c r="A30" s="26">
         <v>29</v>
       </c>
-      <c r="B30" s="37"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="13" t="s">
         <v>58</v>
       </c>
@@ -3763,7 +3763,7 @@
       <c r="W30" s="23">
         <v>1</v>
       </c>
-      <c r="X30" s="42">
+      <c r="X30" s="35">
         <v>0</v>
       </c>
       <c r="Y30" s="23">
@@ -3780,7 +3780,7 @@
       <c r="A31" s="26">
         <v>30</v>
       </c>
-      <c r="B31" s="36"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="13" t="s">
         <v>59</v>
       </c>
@@ -3847,7 +3847,7 @@
       <c r="X31" s="23">
         <v>1</v>
       </c>
-      <c r="Y31" s="42">
+      <c r="Y31" s="35">
         <v>0</v>
       </c>
       <c r="Z31" s="7"/>
@@ -3861,7 +3861,7 @@
       <c r="A32" s="26">
         <v>31</v>
       </c>
-      <c r="B32" s="41"/>
+      <c r="B32" s="37"/>
       <c r="C32" s="3" t="s">
         <v>50</v>
       </c>
@@ -3928,7 +3928,7 @@
       <c r="X32" s="23">
         <v>0.5</v>
       </c>
-      <c r="Y32" s="42">
+      <c r="Y32" s="35">
         <v>0</v>
       </c>
       <c r="Z32" s="7"/>
@@ -4009,7 +4009,7 @@
       <c r="X33" s="23">
         <v>0.5</v>
       </c>
-      <c r="Y33" s="42">
+      <c r="Y33" s="35">
         <v>0</v>
       </c>
       <c r="Z33" s="7"/>
@@ -4090,7 +4090,7 @@
       <c r="X34" s="23">
         <v>0.5</v>
       </c>
-      <c r="Y34" s="42">
+      <c r="Y34" s="35">
         <v>0</v>
       </c>
       <c r="Z34" s="7"/>
@@ -4171,7 +4171,7 @@
       <c r="X35" s="23">
         <v>0.5</v>
       </c>
-      <c r="Y35" s="42">
+      <c r="Y35" s="35">
         <v>0</v>
       </c>
       <c r="Z35" s="7"/>
@@ -4252,7 +4252,7 @@
       <c r="X36" s="23">
         <v>0.5</v>
       </c>
-      <c r="Y36" s="42">
+      <c r="Y36" s="35">
         <v>0</v>
       </c>
       <c r="Z36" s="7"/>
@@ -4333,7 +4333,7 @@
       <c r="X37" s="23">
         <v>0.5</v>
       </c>
-      <c r="Y37" s="42">
+      <c r="Y37" s="35">
         <v>0</v>
       </c>
       <c r="Z37" s="7"/>
@@ -4767,16 +4767,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B17:B20"/>
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="B25:B28"/>
     <mergeCell ref="B32:B37"/>
     <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4787,8 +4787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4915,24 +4915,24 @@
       </c>
       <c r="F2" s="32"/>
       <c r="G2" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H2" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I2" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J2" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K2" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L2" s="23">
-        <v>0</v>
-      </c>
-      <c r="M2" s="23">
+        <v>5</v>
+      </c>
+      <c r="M2" s="35">
         <v>0</v>
       </c>
       <c r="N2" s="23">
@@ -4979,7 +4979,7 @@
       <c r="A3" s="26">
         <v>2</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="42" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -4993,24 +4993,24 @@
       </c>
       <c r="F3" s="32"/>
       <c r="G3" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H3" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I3" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J3" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K3" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L3" s="23">
-        <v>0</v>
-      </c>
-      <c r="M3" s="23">
+        <v>4</v>
+      </c>
+      <c r="M3" s="35">
         <v>0</v>
       </c>
       <c r="N3" s="23">
@@ -5057,7 +5057,7 @@
       <c r="A4" s="26">
         <v>3</v>
       </c>
-      <c r="B4" s="36"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="16" t="s">
         <v>20</v>
       </c>
@@ -5069,24 +5069,24 @@
       </c>
       <c r="F4" s="32"/>
       <c r="G4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L4" s="23">
-        <v>0</v>
-      </c>
-      <c r="M4" s="23">
+        <v>6</v>
+      </c>
+      <c r="M4" s="35">
         <v>0</v>
       </c>
       <c r="N4" s="23">
@@ -5133,7 +5133,7 @@
       <c r="A5" s="26">
         <v>4</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="42" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="29" t="s">
@@ -5147,24 +5147,24 @@
       </c>
       <c r="F5" s="32"/>
       <c r="G5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="23">
-        <v>0</v>
-      </c>
-      <c r="M5" s="23">
+        <v>1</v>
+      </c>
+      <c r="M5" s="35">
         <v>0</v>
       </c>
       <c r="N5" s="23">
@@ -5211,7 +5211,7 @@
       <c r="A6" s="26">
         <v>5</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="13" t="s">
         <v>14</v>
       </c>
@@ -5223,24 +5223,24 @@
       </c>
       <c r="F6" s="32"/>
       <c r="G6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L6" s="23">
-        <v>0</v>
-      </c>
-      <c r="M6" s="23">
+        <v>8</v>
+      </c>
+      <c r="M6" s="35">
         <v>0</v>
       </c>
       <c r="N6" s="23">
@@ -5287,7 +5287,7 @@
       <c r="A7" s="26">
         <v>6</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="42" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -5301,24 +5301,24 @@
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L7" s="23">
-        <v>0</v>
-      </c>
-      <c r="M7" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M7" s="35">
         <v>0</v>
       </c>
       <c r="N7" s="23">
@@ -5365,7 +5365,7 @@
       <c r="A8" s="26">
         <v>7</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="13" t="s">
         <v>22</v>
       </c>
@@ -5377,24 +5377,24 @@
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="23">
-        <v>0</v>
-      </c>
-      <c r="M8" s="23">
+        <v>1</v>
+      </c>
+      <c r="M8" s="35">
         <v>0</v>
       </c>
       <c r="N8" s="23">
@@ -5441,7 +5441,7 @@
       <c r="A9" s="26">
         <v>8</v>
       </c>
-      <c r="B9" s="36"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="13" t="s">
         <v>15</v>
       </c>
@@ -5453,24 +5453,24 @@
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="23">
-        <v>0</v>
-      </c>
-      <c r="M9" s="23">
+        <v>1</v>
+      </c>
+      <c r="M9" s="35">
         <v>0</v>
       </c>
       <c r="N9" s="23">
@@ -5517,7 +5517,7 @@
       <c r="A10" s="26">
         <v>9</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="42" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -5531,24 +5531,24 @@
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L10" s="23">
-        <v>0</v>
-      </c>
-      <c r="M10" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="35">
         <v>0</v>
       </c>
       <c r="N10" s="23">
@@ -5595,7 +5595,7 @@
       <c r="A11" s="26">
         <v>10</v>
       </c>
-      <c r="B11" s="37"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="13" t="s">
         <v>29</v>
       </c>
@@ -5607,24 +5607,24 @@
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L11" s="23">
-        <v>0</v>
-      </c>
-      <c r="M11" s="23">
+        <v>4</v>
+      </c>
+      <c r="M11" s="35">
         <v>0</v>
       </c>
       <c r="N11" s="23">
@@ -5671,7 +5671,7 @@
       <c r="A12" s="26">
         <v>11</v>
       </c>
-      <c r="B12" s="37"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="17" t="s">
         <v>30</v>
       </c>
@@ -5683,24 +5683,24 @@
       </c>
       <c r="F12" s="32"/>
       <c r="G12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L12" s="23">
-        <v>0</v>
-      </c>
-      <c r="M12" s="23">
+        <v>2</v>
+      </c>
+      <c r="M12" s="35">
         <v>0</v>
       </c>
       <c r="N12" s="23">
@@ -5747,7 +5747,7 @@
       <c r="A13" s="26">
         <v>12</v>
       </c>
-      <c r="B13" s="36"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="17" t="s">
         <v>31</v>
       </c>
@@ -5759,24 +5759,24 @@
       </c>
       <c r="F13" s="32"/>
       <c r="G13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L13" s="23">
-        <v>0</v>
-      </c>
-      <c r="M13" s="23">
+        <v>4</v>
+      </c>
+      <c r="M13" s="35">
         <v>0</v>
       </c>
       <c r="N13" s="23">
@@ -5823,7 +5823,7 @@
       <c r="A14" s="26">
         <v>13</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="42" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -5837,24 +5837,24 @@
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="23">
-        <v>0</v>
-      </c>
-      <c r="M14" s="23">
+        <v>1</v>
+      </c>
+      <c r="M14" s="35">
         <v>0</v>
       </c>
       <c r="N14" s="23">
@@ -5913,24 +5913,24 @@
       </c>
       <c r="F15" s="32"/>
       <c r="G15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L15" s="23">
-        <v>0</v>
-      </c>
-      <c r="M15" s="23">
+        <v>2</v>
+      </c>
+      <c r="M15" s="35">
         <v>0</v>
       </c>
       <c r="N15" s="23">
@@ -5989,24 +5989,24 @@
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L16" s="23">
-        <v>0</v>
-      </c>
-      <c r="M16" s="23">
+        <v>4</v>
+      </c>
+      <c r="M16" s="35">
         <v>0</v>
       </c>
       <c r="N16" s="23">
@@ -6053,7 +6053,7 @@
       <c r="A17" s="26">
         <v>16</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="36" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -6067,24 +6067,24 @@
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" s="23">
-        <v>0</v>
-      </c>
-      <c r="M17" s="23">
+        <v>1</v>
+      </c>
+      <c r="M17" s="35">
         <v>0</v>
       </c>
       <c r="N17" s="23">
@@ -6131,7 +6131,7 @@
       <c r="A18" s="26">
         <v>17</v>
       </c>
-      <c r="B18" s="40"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="13" t="s">
         <v>38</v>
       </c>
@@ -6143,24 +6143,24 @@
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L18" s="23">
-        <v>0</v>
-      </c>
-      <c r="M18" s="23">
+        <v>2</v>
+      </c>
+      <c r="M18" s="35">
         <v>0</v>
       </c>
       <c r="N18" s="23">
@@ -6207,7 +6207,7 @@
       <c r="A19" s="26">
         <v>18</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="13" t="s">
         <v>39</v>
       </c>
@@ -6219,24 +6219,24 @@
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L19" s="23">
-        <v>0</v>
-      </c>
-      <c r="M19" s="23">
+        <v>2</v>
+      </c>
+      <c r="M19" s="35">
         <v>0</v>
       </c>
       <c r="N19" s="23">
@@ -6283,7 +6283,7 @@
       <c r="A20" s="26">
         <v>19</v>
       </c>
-      <c r="B20" s="40"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="12" t="s">
         <v>40</v>
       </c>
@@ -6295,24 +6295,24 @@
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L20" s="23">
-        <v>0</v>
-      </c>
-      <c r="M20" s="23">
+        <v>5</v>
+      </c>
+      <c r="M20" s="35">
         <v>0</v>
       </c>
       <c r="N20" s="23">
@@ -6359,7 +6359,7 @@
       <c r="A21" s="26">
         <v>20</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="36" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -6373,24 +6373,24 @@
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" s="23">
-        <v>0</v>
-      </c>
-      <c r="M21" s="23">
+        <v>1</v>
+      </c>
+      <c r="M21" s="35">
         <v>0</v>
       </c>
       <c r="N21" s="23">
@@ -6437,7 +6437,7 @@
       <c r="A22" s="26">
         <v>21</v>
       </c>
-      <c r="B22" s="40"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="13" t="s">
         <v>43</v>
       </c>
@@ -6449,24 +6449,24 @@
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" s="23">
-        <v>0</v>
-      </c>
-      <c r="M22" s="23">
+        <v>1</v>
+      </c>
+      <c r="M22" s="35">
         <v>0</v>
       </c>
       <c r="N22" s="23">
@@ -6513,7 +6513,7 @@
       <c r="A23" s="26">
         <v>22</v>
       </c>
-      <c r="B23" s="40"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="13" t="s">
         <v>44</v>
       </c>
@@ -6525,24 +6525,24 @@
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L23" s="23">
-        <v>0</v>
-      </c>
-      <c r="M23" s="23">
+        <v>2</v>
+      </c>
+      <c r="M23" s="35">
         <v>0</v>
       </c>
       <c r="N23" s="23">
@@ -6589,7 +6589,7 @@
       <c r="A24" s="26">
         <v>23</v>
       </c>
-      <c r="B24" s="40"/>
+      <c r="B24" s="36"/>
       <c r="C24" s="12" t="s">
         <v>45</v>
       </c>
@@ -6601,24 +6601,24 @@
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L24" s="23">
-        <v>0</v>
-      </c>
-      <c r="M24" s="23">
+        <v>2</v>
+      </c>
+      <c r="M24" s="35">
         <v>0</v>
       </c>
       <c r="N24" s="23">
@@ -6665,7 +6665,7 @@
       <c r="A25" s="26">
         <v>24</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="36" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -6679,24 +6679,24 @@
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L25" s="23">
-        <v>0</v>
-      </c>
-      <c r="M25" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M25" s="35">
         <v>0</v>
       </c>
       <c r="N25" s="23">
@@ -6743,7 +6743,7 @@
       <c r="A26" s="26">
         <v>25</v>
       </c>
-      <c r="B26" s="40"/>
+      <c r="B26" s="36"/>
       <c r="C26" s="13" t="s">
         <v>47</v>
       </c>
@@ -6755,24 +6755,24 @@
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26" s="23">
-        <v>0</v>
-      </c>
-      <c r="M26" s="23">
+        <v>1</v>
+      </c>
+      <c r="M26" s="35">
         <v>0</v>
       </c>
       <c r="N26" s="23">
@@ -6819,7 +6819,7 @@
       <c r="A27" s="26">
         <v>26</v>
       </c>
-      <c r="B27" s="40"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="13" t="s">
         <v>48</v>
       </c>
@@ -6831,24 +6831,24 @@
       </c>
       <c r="F27" s="32"/>
       <c r="G27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L27" s="23">
-        <v>0</v>
-      </c>
-      <c r="M27" s="23">
+        <v>2</v>
+      </c>
+      <c r="M27" s="35">
         <v>0</v>
       </c>
       <c r="N27" s="23">
@@ -6895,7 +6895,7 @@
       <c r="A28" s="26">
         <v>27</v>
       </c>
-      <c r="B28" s="40"/>
+      <c r="B28" s="36"/>
       <c r="C28" s="12" t="s">
         <v>49</v>
       </c>
@@ -6907,24 +6907,24 @@
       </c>
       <c r="F28" s="32"/>
       <c r="G28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L28" s="23">
-        <v>0</v>
-      </c>
-      <c r="M28" s="23">
+        <v>4</v>
+      </c>
+      <c r="M28" s="35">
         <v>0</v>
       </c>
       <c r="N28" s="23">
@@ -6971,7 +6971,7 @@
       <c r="A29" s="26">
         <v>28</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="40" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="13" t="s">
@@ -6985,24 +6985,24 @@
       </c>
       <c r="F29" s="32"/>
       <c r="G29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L29" s="23">
-        <v>0</v>
-      </c>
-      <c r="M29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M29" s="35">
         <v>0</v>
       </c>
       <c r="N29" s="23">
@@ -7049,7 +7049,7 @@
       <c r="A30" s="26">
         <v>29</v>
       </c>
-      <c r="B30" s="37"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="13" t="s">
         <v>58</v>
       </c>
@@ -7061,24 +7061,24 @@
       </c>
       <c r="F30" s="32"/>
       <c r="G30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="23">
-        <v>0</v>
-      </c>
-      <c r="M30" s="23">
+        <v>1</v>
+      </c>
+      <c r="M30" s="35">
         <v>0</v>
       </c>
       <c r="N30" s="23">
@@ -7125,7 +7125,7 @@
       <c r="A31" s="26">
         <v>30</v>
       </c>
-      <c r="B31" s="36"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="13" t="s">
         <v>59</v>
       </c>
@@ -7137,24 +7137,24 @@
       </c>
       <c r="F31" s="32"/>
       <c r="G31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L31" s="23">
-        <v>0</v>
-      </c>
-      <c r="M31" s="23">
+        <v>4</v>
+      </c>
+      <c r="M31" s="35">
         <v>0</v>
       </c>
       <c r="N31" s="23">
@@ -7201,7 +7201,7 @@
       <c r="A32" s="26">
         <v>31</v>
       </c>
-      <c r="B32" s="41"/>
+      <c r="B32" s="37"/>
       <c r="C32" s="3" t="s">
         <v>50</v>
       </c>
@@ -7213,24 +7213,24 @@
       </c>
       <c r="F32" s="32"/>
       <c r="G32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L32" s="23">
-        <v>0</v>
-      </c>
-      <c r="M32" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M32" s="35">
         <v>0</v>
       </c>
       <c r="N32" s="23">
@@ -7289,24 +7289,24 @@
       </c>
       <c r="F33" s="32"/>
       <c r="G33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L33" s="23">
-        <v>0</v>
-      </c>
-      <c r="M33" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M33" s="35">
         <v>0</v>
       </c>
       <c r="N33" s="23">
@@ -7365,24 +7365,24 @@
       </c>
       <c r="F34" s="32"/>
       <c r="G34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L34" s="23">
-        <v>0</v>
-      </c>
-      <c r="M34" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M34" s="35">
         <v>0</v>
       </c>
       <c r="N34" s="23">
@@ -7441,24 +7441,24 @@
       </c>
       <c r="F35" s="32"/>
       <c r="G35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L35" s="23">
-        <v>0</v>
-      </c>
-      <c r="M35" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M35" s="35">
         <v>0</v>
       </c>
       <c r="N35" s="23">
@@ -7517,24 +7517,24 @@
       </c>
       <c r="F36" s="32"/>
       <c r="G36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L36" s="23">
-        <v>0</v>
-      </c>
-      <c r="M36" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M36" s="35">
         <v>0</v>
       </c>
       <c r="N36" s="23">
@@ -7593,24 +7593,24 @@
       </c>
       <c r="F37" s="32"/>
       <c r="G37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L37" s="23">
-        <v>0</v>
-      </c>
-      <c r="M37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="M37" s="35">
         <v>0</v>
       </c>
       <c r="N37" s="23">
@@ -8041,27 +8041,27 @@
       </c>
       <c r="G43" s="25">
         <f>SUM(G7:G41)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="H43" s="25">
         <f t="shared" ref="H43:Z43" si="0">SUM(H7:H41)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="I43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="J43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="K43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="L43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="M43" s="25">
         <f t="shared" si="0"/>
@@ -8122,16 +8122,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B17:B20"/>
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="B25:B28"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B32:B37"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
up time sprint 2
</commit_message>
<xml_diff>
--- a/7.Print-Backlog/Sprint-2.xlsx
+++ b/7.Print-Backlog/Sprint-2.xlsx
@@ -525,11 +525,14 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -537,14 +540,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -850,7 +850,7 @@
                   <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -906,11 +906,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="189969920"/>
-        <c:axId val="189971456"/>
+        <c:axId val="136427008"/>
+        <c:axId val="136428544"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="189969920"/>
+        <c:axId val="136427008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,14 +920,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189971456"/>
+        <c:crossAx val="136428544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="189971456"/>
+        <c:axId val="136428544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,7 +938,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="189969920"/>
+        <c:crossAx val="136427008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1494,7 +1494,7 @@
       <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="36" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -1577,7 +1577,7 @@
       <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="16" t="s">
         <v>20</v>
       </c>
@@ -1658,7 +1658,7 @@
       <c r="A5" s="26">
         <v>4</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="36" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="29" t="s">
@@ -1741,7 +1741,7 @@
       <c r="A6" s="26">
         <v>5</v>
       </c>
-      <c r="B6" s="41"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="13" t="s">
         <v>14</v>
       </c>
@@ -1822,7 +1822,7 @@
       <c r="A7" s="26">
         <v>6</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -1905,7 +1905,7 @@
       <c r="A8" s="26">
         <v>7</v>
       </c>
-      <c r="B8" s="40"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="13" t="s">
         <v>22</v>
       </c>
@@ -1986,7 +1986,7 @@
       <c r="A9" s="26">
         <v>8</v>
       </c>
-      <c r="B9" s="41"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="13" t="s">
         <v>15</v>
       </c>
@@ -2067,7 +2067,7 @@
       <c r="A10" s="26">
         <v>9</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -2150,7 +2150,7 @@
       <c r="A11" s="26">
         <v>10</v>
       </c>
-      <c r="B11" s="40"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="13" t="s">
         <v>29</v>
       </c>
@@ -2231,7 +2231,7 @@
       <c r="A12" s="26">
         <v>11</v>
       </c>
-      <c r="B12" s="40"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="17" t="s">
         <v>30</v>
       </c>
@@ -2312,7 +2312,7 @@
       <c r="A13" s="26">
         <v>12</v>
       </c>
-      <c r="B13" s="41"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="17" t="s">
         <v>31</v>
       </c>
@@ -2393,7 +2393,7 @@
       <c r="A14" s="26">
         <v>13</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="36" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -2476,7 +2476,7 @@
       <c r="A15" s="26">
         <v>14</v>
       </c>
-      <c r="B15" s="38"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="13" t="s">
         <v>34</v>
       </c>
@@ -2557,7 +2557,7 @@
       <c r="A16" s="26">
         <v>15</v>
       </c>
-      <c r="B16" s="39"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="13" t="s">
         <v>35</v>
       </c>
@@ -2638,7 +2638,7 @@
       <c r="A17" s="26">
         <v>16</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="41" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -2721,7 +2721,7 @@
       <c r="A18" s="26">
         <v>17</v>
       </c>
-      <c r="B18" s="36"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="13" t="s">
         <v>38</v>
       </c>
@@ -2802,7 +2802,7 @@
       <c r="A19" s="26">
         <v>18</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="13" t="s">
         <v>39</v>
       </c>
@@ -2883,7 +2883,7 @@
       <c r="A20" s="26">
         <v>19</v>
       </c>
-      <c r="B20" s="36"/>
+      <c r="B20" s="41"/>
       <c r="C20" s="12" t="s">
         <v>40</v>
       </c>
@@ -2964,7 +2964,7 @@
       <c r="A21" s="26">
         <v>20</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="41" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -3047,7 +3047,7 @@
       <c r="A22" s="26">
         <v>21</v>
       </c>
-      <c r="B22" s="36"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="13" t="s">
         <v>43</v>
       </c>
@@ -3128,7 +3128,7 @@
       <c r="A23" s="26">
         <v>22</v>
       </c>
-      <c r="B23" s="36"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="13" t="s">
         <v>44</v>
       </c>
@@ -3209,7 +3209,7 @@
       <c r="A24" s="26">
         <v>23</v>
       </c>
-      <c r="B24" s="36"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="12" t="s">
         <v>45</v>
       </c>
@@ -3290,7 +3290,7 @@
       <c r="A25" s="26">
         <v>24</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="41" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -3373,7 +3373,7 @@
       <c r="A26" s="26">
         <v>25</v>
       </c>
-      <c r="B26" s="36"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="13" t="s">
         <v>47</v>
       </c>
@@ -3454,7 +3454,7 @@
       <c r="A27" s="26">
         <v>26</v>
       </c>
-      <c r="B27" s="36"/>
+      <c r="B27" s="41"/>
       <c r="C27" s="13" t="s">
         <v>48</v>
       </c>
@@ -3535,7 +3535,7 @@
       <c r="A28" s="26">
         <v>27</v>
       </c>
-      <c r="B28" s="36"/>
+      <c r="B28" s="41"/>
       <c r="C28" s="12" t="s">
         <v>49</v>
       </c>
@@ -3616,7 +3616,7 @@
       <c r="A29" s="26">
         <v>28</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="38" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="13" t="s">
@@ -3699,7 +3699,7 @@
       <c r="A30" s="26">
         <v>29</v>
       </c>
-      <c r="B30" s="40"/>
+      <c r="B30" s="38"/>
       <c r="C30" s="13" t="s">
         <v>58</v>
       </c>
@@ -3780,7 +3780,7 @@
       <c r="A31" s="26">
         <v>30</v>
       </c>
-      <c r="B31" s="41"/>
+      <c r="B31" s="37"/>
       <c r="C31" s="13" t="s">
         <v>59</v>
       </c>
@@ -3861,7 +3861,7 @@
       <c r="A32" s="26">
         <v>31</v>
       </c>
-      <c r="B32" s="37"/>
+      <c r="B32" s="42"/>
       <c r="C32" s="3" t="s">
         <v>50</v>
       </c>
@@ -3942,7 +3942,7 @@
       <c r="A33" s="26">
         <v>32</v>
       </c>
-      <c r="B33" s="38"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="3" t="s">
         <v>51</v>
       </c>
@@ -4023,7 +4023,7 @@
       <c r="A34" s="26">
         <v>33</v>
       </c>
-      <c r="B34" s="38"/>
+      <c r="B34" s="39"/>
       <c r="C34" s="3" t="s">
         <v>52</v>
       </c>
@@ -4104,7 +4104,7 @@
       <c r="A35" s="26">
         <v>34</v>
       </c>
-      <c r="B35" s="38"/>
+      <c r="B35" s="39"/>
       <c r="C35" s="3" t="s">
         <v>53</v>
       </c>
@@ -4185,7 +4185,7 @@
       <c r="A36" s="26">
         <v>35</v>
       </c>
-      <c r="B36" s="38"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="12" t="s">
         <v>54</v>
       </c>
@@ -4266,7 +4266,7 @@
       <c r="A37" s="26">
         <v>36</v>
       </c>
-      <c r="B37" s="39"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="12" t="s">
         <v>60</v>
       </c>
@@ -4767,16 +4767,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="B29:B31"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="B29:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4787,8 +4787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="E16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4932,10 +4932,10 @@
       <c r="L2" s="23">
         <v>5</v>
       </c>
-      <c r="M2" s="35">
-        <v>0</v>
-      </c>
-      <c r="N2" s="23">
+      <c r="M2" s="23">
+        <v>5</v>
+      </c>
+      <c r="N2" s="35">
         <v>0</v>
       </c>
       <c r="O2" s="23">
@@ -4979,7 +4979,7 @@
       <c r="A3" s="26">
         <v>2</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="36" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -5010,10 +5010,10 @@
       <c r="L3" s="23">
         <v>4</v>
       </c>
-      <c r="M3" s="35">
-        <v>0</v>
-      </c>
-      <c r="N3" s="23">
+      <c r="M3" s="23">
+        <v>4</v>
+      </c>
+      <c r="N3" s="35">
         <v>0</v>
       </c>
       <c r="O3" s="23">
@@ -5057,7 +5057,7 @@
       <c r="A4" s="26">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="16" t="s">
         <v>20</v>
       </c>
@@ -5086,10 +5086,10 @@
       <c r="L4" s="23">
         <v>6</v>
       </c>
-      <c r="M4" s="35">
-        <v>0</v>
-      </c>
-      <c r="N4" s="23">
+      <c r="M4" s="23">
+        <v>6</v>
+      </c>
+      <c r="N4" s="35">
         <v>0</v>
       </c>
       <c r="O4" s="23">
@@ -5133,7 +5133,7 @@
       <c r="A5" s="26">
         <v>4</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="36" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="29" t="s">
@@ -5164,10 +5164,10 @@
       <c r="L5" s="23">
         <v>1</v>
       </c>
-      <c r="M5" s="35">
-        <v>0</v>
-      </c>
-      <c r="N5" s="23">
+      <c r="M5" s="23">
+        <v>1</v>
+      </c>
+      <c r="N5" s="35">
         <v>0</v>
       </c>
       <c r="O5" s="23">
@@ -5211,7 +5211,7 @@
       <c r="A6" s="26">
         <v>5</v>
       </c>
-      <c r="B6" s="41"/>
+      <c r="B6" s="37"/>
       <c r="C6" s="13" t="s">
         <v>14</v>
       </c>
@@ -5240,10 +5240,10 @@
       <c r="L6" s="23">
         <v>8</v>
       </c>
-      <c r="M6" s="35">
-        <v>0</v>
-      </c>
-      <c r="N6" s="23">
+      <c r="M6" s="23">
+        <v>8</v>
+      </c>
+      <c r="N6" s="35">
         <v>0</v>
       </c>
       <c r="O6" s="23">
@@ -5287,7 +5287,7 @@
       <c r="A7" s="26">
         <v>6</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -5318,10 +5318,10 @@
       <c r="L7" s="23">
         <v>0.5</v>
       </c>
-      <c r="M7" s="35">
-        <v>0</v>
-      </c>
-      <c r="N7" s="23">
+      <c r="M7" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="N7" s="35">
         <v>0</v>
       </c>
       <c r="O7" s="23">
@@ -5365,7 +5365,7 @@
       <c r="A8" s="26">
         <v>7</v>
       </c>
-      <c r="B8" s="40"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="13" t="s">
         <v>22</v>
       </c>
@@ -5394,10 +5394,10 @@
       <c r="L8" s="23">
         <v>1</v>
       </c>
-      <c r="M8" s="35">
-        <v>0</v>
-      </c>
-      <c r="N8" s="23">
+      <c r="M8" s="23">
+        <v>1</v>
+      </c>
+      <c r="N8" s="35">
         <v>0</v>
       </c>
       <c r="O8" s="23">
@@ -5441,7 +5441,7 @@
       <c r="A9" s="26">
         <v>8</v>
       </c>
-      <c r="B9" s="41"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="13" t="s">
         <v>15</v>
       </c>
@@ -5470,10 +5470,10 @@
       <c r="L9" s="23">
         <v>1</v>
       </c>
-      <c r="M9" s="35">
-        <v>0</v>
-      </c>
-      <c r="N9" s="23">
+      <c r="M9" s="23">
+        <v>1</v>
+      </c>
+      <c r="N9" s="35">
         <v>0</v>
       </c>
       <c r="O9" s="23">
@@ -5517,7 +5517,7 @@
       <c r="A10" s="26">
         <v>9</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -5548,10 +5548,10 @@
       <c r="L10" s="23">
         <v>0.5</v>
       </c>
-      <c r="M10" s="35">
-        <v>0</v>
-      </c>
-      <c r="N10" s="23">
+      <c r="M10" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="N10" s="35">
         <v>0</v>
       </c>
       <c r="O10" s="23">
@@ -5595,7 +5595,7 @@
       <c r="A11" s="26">
         <v>10</v>
       </c>
-      <c r="B11" s="40"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="13" t="s">
         <v>29</v>
       </c>
@@ -5624,10 +5624,10 @@
       <c r="L11" s="23">
         <v>4</v>
       </c>
-      <c r="M11" s="35">
-        <v>0</v>
-      </c>
-      <c r="N11" s="23">
+      <c r="M11" s="23">
+        <v>4</v>
+      </c>
+      <c r="N11" s="35">
         <v>0</v>
       </c>
       <c r="O11" s="23">
@@ -5671,7 +5671,7 @@
       <c r="A12" s="26">
         <v>11</v>
       </c>
-      <c r="B12" s="40"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="17" t="s">
         <v>30</v>
       </c>
@@ -5700,10 +5700,10 @@
       <c r="L12" s="23">
         <v>2</v>
       </c>
-      <c r="M12" s="35">
-        <v>0</v>
-      </c>
-      <c r="N12" s="23">
+      <c r="M12" s="23">
+        <v>2</v>
+      </c>
+      <c r="N12" s="35">
         <v>0</v>
       </c>
       <c r="O12" s="23">
@@ -5747,7 +5747,7 @@
       <c r="A13" s="26">
         <v>12</v>
       </c>
-      <c r="B13" s="41"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="17" t="s">
         <v>31</v>
       </c>
@@ -5776,10 +5776,10 @@
       <c r="L13" s="23">
         <v>4</v>
       </c>
-      <c r="M13" s="35">
-        <v>0</v>
-      </c>
-      <c r="N13" s="23">
+      <c r="M13" s="23">
+        <v>4</v>
+      </c>
+      <c r="N13" s="35">
         <v>0</v>
       </c>
       <c r="O13" s="23">
@@ -5823,7 +5823,7 @@
       <c r="A14" s="26">
         <v>13</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="36" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -5854,10 +5854,10 @@
       <c r="L14" s="23">
         <v>1</v>
       </c>
-      <c r="M14" s="35">
-        <v>0</v>
-      </c>
-      <c r="N14" s="23">
+      <c r="M14" s="23">
+        <v>1</v>
+      </c>
+      <c r="N14" s="35">
         <v>0</v>
       </c>
       <c r="O14" s="23">
@@ -5901,7 +5901,7 @@
       <c r="A15" s="26">
         <v>14</v>
       </c>
-      <c r="B15" s="38"/>
+      <c r="B15" s="39"/>
       <c r="C15" s="13" t="s">
         <v>34</v>
       </c>
@@ -5930,10 +5930,10 @@
       <c r="L15" s="23">
         <v>2</v>
       </c>
-      <c r="M15" s="35">
-        <v>0</v>
-      </c>
-      <c r="N15" s="23">
+      <c r="M15" s="23">
+        <v>2</v>
+      </c>
+      <c r="N15" s="35">
         <v>0</v>
       </c>
       <c r="O15" s="23">
@@ -5977,7 +5977,7 @@
       <c r="A16" s="26">
         <v>15</v>
       </c>
-      <c r="B16" s="39"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="13" t="s">
         <v>35</v>
       </c>
@@ -6006,10 +6006,10 @@
       <c r="L16" s="23">
         <v>4</v>
       </c>
-      <c r="M16" s="35">
-        <v>0</v>
-      </c>
-      <c r="N16" s="23">
+      <c r="M16" s="23">
+        <v>4</v>
+      </c>
+      <c r="N16" s="35">
         <v>0</v>
       </c>
       <c r="O16" s="23">
@@ -6053,7 +6053,7 @@
       <c r="A17" s="26">
         <v>16</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="41" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -6084,10 +6084,10 @@
       <c r="L17" s="23">
         <v>1</v>
       </c>
-      <c r="M17" s="35">
-        <v>0</v>
-      </c>
-      <c r="N17" s="23">
+      <c r="M17" s="23">
+        <v>1</v>
+      </c>
+      <c r="N17" s="35">
         <v>0</v>
       </c>
       <c r="O17" s="23">
@@ -6131,7 +6131,7 @@
       <c r="A18" s="26">
         <v>17</v>
       </c>
-      <c r="B18" s="36"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="13" t="s">
         <v>38</v>
       </c>
@@ -6160,10 +6160,10 @@
       <c r="L18" s="23">
         <v>2</v>
       </c>
-      <c r="M18" s="35">
-        <v>0</v>
-      </c>
-      <c r="N18" s="23">
+      <c r="M18" s="23">
+        <v>2</v>
+      </c>
+      <c r="N18" s="35">
         <v>0</v>
       </c>
       <c r="O18" s="23">
@@ -6207,7 +6207,7 @@
       <c r="A19" s="26">
         <v>18</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="13" t="s">
         <v>39</v>
       </c>
@@ -6236,10 +6236,10 @@
       <c r="L19" s="23">
         <v>2</v>
       </c>
-      <c r="M19" s="35">
-        <v>0</v>
-      </c>
-      <c r="N19" s="23">
+      <c r="M19" s="23">
+        <v>2</v>
+      </c>
+      <c r="N19" s="35">
         <v>0</v>
       </c>
       <c r="O19" s="23">
@@ -6283,7 +6283,7 @@
       <c r="A20" s="26">
         <v>19</v>
       </c>
-      <c r="B20" s="36"/>
+      <c r="B20" s="41"/>
       <c r="C20" s="12" t="s">
         <v>40</v>
       </c>
@@ -6312,10 +6312,10 @@
       <c r="L20" s="23">
         <v>5</v>
       </c>
-      <c r="M20" s="35">
-        <v>0</v>
-      </c>
-      <c r="N20" s="23">
+      <c r="M20" s="23">
+        <v>5</v>
+      </c>
+      <c r="N20" s="35">
         <v>0</v>
       </c>
       <c r="O20" s="23">
@@ -6359,7 +6359,7 @@
       <c r="A21" s="26">
         <v>20</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="41" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -6390,10 +6390,10 @@
       <c r="L21" s="23">
         <v>1</v>
       </c>
-      <c r="M21" s="35">
-        <v>0</v>
-      </c>
-      <c r="N21" s="23">
+      <c r="M21" s="23">
+        <v>1</v>
+      </c>
+      <c r="N21" s="35">
         <v>0</v>
       </c>
       <c r="O21" s="23">
@@ -6437,7 +6437,7 @@
       <c r="A22" s="26">
         <v>21</v>
       </c>
-      <c r="B22" s="36"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="13" t="s">
         <v>43</v>
       </c>
@@ -6466,10 +6466,10 @@
       <c r="L22" s="23">
         <v>1</v>
       </c>
-      <c r="M22" s="35">
-        <v>0</v>
-      </c>
-      <c r="N22" s="23">
+      <c r="M22" s="23">
+        <v>1</v>
+      </c>
+      <c r="N22" s="35">
         <v>0</v>
       </c>
       <c r="O22" s="23">
@@ -6513,7 +6513,7 @@
       <c r="A23" s="26">
         <v>22</v>
       </c>
-      <c r="B23" s="36"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="13" t="s">
         <v>44</v>
       </c>
@@ -6542,10 +6542,10 @@
       <c r="L23" s="23">
         <v>2</v>
       </c>
-      <c r="M23" s="35">
-        <v>0</v>
-      </c>
-      <c r="N23" s="23">
+      <c r="M23" s="23">
+        <v>2</v>
+      </c>
+      <c r="N23" s="35">
         <v>0</v>
       </c>
       <c r="O23" s="23">
@@ -6589,7 +6589,7 @@
       <c r="A24" s="26">
         <v>23</v>
       </c>
-      <c r="B24" s="36"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="12" t="s">
         <v>45</v>
       </c>
@@ -6618,10 +6618,10 @@
       <c r="L24" s="23">
         <v>2</v>
       </c>
-      <c r="M24" s="35">
-        <v>0</v>
-      </c>
-      <c r="N24" s="23">
+      <c r="M24" s="23">
+        <v>2</v>
+      </c>
+      <c r="N24" s="35">
         <v>0</v>
       </c>
       <c r="O24" s="23">
@@ -6665,7 +6665,7 @@
       <c r="A25" s="26">
         <v>24</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="41" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -6696,10 +6696,10 @@
       <c r="L25" s="23">
         <v>0.5</v>
       </c>
-      <c r="M25" s="35">
-        <v>0</v>
-      </c>
-      <c r="N25" s="23">
+      <c r="M25" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="N25" s="35">
         <v>0</v>
       </c>
       <c r="O25" s="23">
@@ -6743,7 +6743,7 @@
       <c r="A26" s="26">
         <v>25</v>
       </c>
-      <c r="B26" s="36"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="13" t="s">
         <v>47</v>
       </c>
@@ -6772,10 +6772,10 @@
       <c r="L26" s="23">
         <v>1</v>
       </c>
-      <c r="M26" s="35">
-        <v>0</v>
-      </c>
-      <c r="N26" s="23">
+      <c r="M26" s="23">
+        <v>1</v>
+      </c>
+      <c r="N26" s="35">
         <v>0</v>
       </c>
       <c r="O26" s="23">
@@ -6819,7 +6819,7 @@
       <c r="A27" s="26">
         <v>26</v>
       </c>
-      <c r="B27" s="36"/>
+      <c r="B27" s="41"/>
       <c r="C27" s="13" t="s">
         <v>48</v>
       </c>
@@ -6848,10 +6848,10 @@
       <c r="L27" s="23">
         <v>2</v>
       </c>
-      <c r="M27" s="35">
-        <v>0</v>
-      </c>
-      <c r="N27" s="23">
+      <c r="M27" s="23">
+        <v>2</v>
+      </c>
+      <c r="N27" s="35">
         <v>0</v>
       </c>
       <c r="O27" s="23">
@@ -6895,7 +6895,7 @@
       <c r="A28" s="26">
         <v>27</v>
       </c>
-      <c r="B28" s="36"/>
+      <c r="B28" s="41"/>
       <c r="C28" s="12" t="s">
         <v>49</v>
       </c>
@@ -6924,10 +6924,10 @@
       <c r="L28" s="23">
         <v>4</v>
       </c>
-      <c r="M28" s="35">
-        <v>0</v>
-      </c>
-      <c r="N28" s="23">
+      <c r="M28" s="23">
+        <v>4</v>
+      </c>
+      <c r="N28" s="35">
         <v>0</v>
       </c>
       <c r="O28" s="23">
@@ -6971,7 +6971,7 @@
       <c r="A29" s="26">
         <v>28</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="38" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="13" t="s">
@@ -7002,10 +7002,10 @@
       <c r="L29" s="23">
         <v>0.5</v>
       </c>
-      <c r="M29" s="35">
-        <v>0</v>
-      </c>
-      <c r="N29" s="23">
+      <c r="M29" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="N29" s="35">
         <v>0</v>
       </c>
       <c r="O29" s="23">
@@ -7049,7 +7049,7 @@
       <c r="A30" s="26">
         <v>29</v>
       </c>
-      <c r="B30" s="40"/>
+      <c r="B30" s="38"/>
       <c r="C30" s="13" t="s">
         <v>58</v>
       </c>
@@ -7078,10 +7078,10 @@
       <c r="L30" s="23">
         <v>1</v>
       </c>
-      <c r="M30" s="35">
-        <v>0</v>
-      </c>
-      <c r="N30" s="23">
+      <c r="M30" s="23">
+        <v>1</v>
+      </c>
+      <c r="N30" s="35">
         <v>0</v>
       </c>
       <c r="O30" s="23">
@@ -7125,7 +7125,7 @@
       <c r="A31" s="26">
         <v>30</v>
       </c>
-      <c r="B31" s="41"/>
+      <c r="B31" s="37"/>
       <c r="C31" s="13" t="s">
         <v>59</v>
       </c>
@@ -7154,10 +7154,10 @@
       <c r="L31" s="23">
         <v>4</v>
       </c>
-      <c r="M31" s="35">
-        <v>0</v>
-      </c>
-      <c r="N31" s="23">
+      <c r="M31" s="23">
+        <v>4</v>
+      </c>
+      <c r="N31" s="35">
         <v>0</v>
       </c>
       <c r="O31" s="23">
@@ -7201,7 +7201,7 @@
       <c r="A32" s="26">
         <v>31</v>
       </c>
-      <c r="B32" s="37"/>
+      <c r="B32" s="42"/>
       <c r="C32" s="3" t="s">
         <v>50</v>
       </c>
@@ -7230,10 +7230,10 @@
       <c r="L32" s="23">
         <v>0.5</v>
       </c>
-      <c r="M32" s="35">
-        <v>0</v>
-      </c>
-      <c r="N32" s="23">
+      <c r="M32" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="N32" s="35">
         <v>0</v>
       </c>
       <c r="O32" s="23">
@@ -7277,7 +7277,7 @@
       <c r="A33" s="26">
         <v>32</v>
       </c>
-      <c r="B33" s="38"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="3" t="s">
         <v>51</v>
       </c>
@@ -7306,10 +7306,10 @@
       <c r="L33" s="23">
         <v>0.5</v>
       </c>
-      <c r="M33" s="35">
-        <v>0</v>
-      </c>
-      <c r="N33" s="23">
+      <c r="M33" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="N33" s="35">
         <v>0</v>
       </c>
       <c r="O33" s="23">
@@ -7353,7 +7353,7 @@
       <c r="A34" s="26">
         <v>33</v>
       </c>
-      <c r="B34" s="38"/>
+      <c r="B34" s="39"/>
       <c r="C34" s="3" t="s">
         <v>52</v>
       </c>
@@ -7382,10 +7382,10 @@
       <c r="L34" s="23">
         <v>0.5</v>
       </c>
-      <c r="M34" s="35">
-        <v>0</v>
-      </c>
-      <c r="N34" s="23">
+      <c r="M34" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="N34" s="35">
         <v>0</v>
       </c>
       <c r="O34" s="23">
@@ -7429,7 +7429,7 @@
       <c r="A35" s="26">
         <v>34</v>
       </c>
-      <c r="B35" s="38"/>
+      <c r="B35" s="39"/>
       <c r="C35" s="3" t="s">
         <v>53</v>
       </c>
@@ -7458,10 +7458,10 @@
       <c r="L35" s="23">
         <v>0.5</v>
       </c>
-      <c r="M35" s="35">
-        <v>0</v>
-      </c>
-      <c r="N35" s="23">
+      <c r="M35" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="N35" s="35">
         <v>0</v>
       </c>
       <c r="O35" s="23">
@@ -7505,7 +7505,7 @@
       <c r="A36" s="26">
         <v>35</v>
       </c>
-      <c r="B36" s="38"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="12" t="s">
         <v>54</v>
       </c>
@@ -7534,10 +7534,10 @@
       <c r="L36" s="23">
         <v>0.5</v>
       </c>
-      <c r="M36" s="35">
-        <v>0</v>
-      </c>
-      <c r="N36" s="23">
+      <c r="M36" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="N36" s="35">
         <v>0</v>
       </c>
       <c r="O36" s="23">
@@ -7581,7 +7581,7 @@
       <c r="A37" s="26">
         <v>36</v>
       </c>
-      <c r="B37" s="39"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="12" t="s">
         <v>60</v>
       </c>
@@ -7610,10 +7610,10 @@
       <c r="L37" s="23">
         <v>0.5</v>
       </c>
-      <c r="M37" s="35">
-        <v>0</v>
-      </c>
-      <c r="N37" s="23">
+      <c r="M37" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="N37" s="35">
         <v>0</v>
       </c>
       <c r="O37" s="23">
@@ -8065,7 +8065,7 @@
       </c>
       <c r="M43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="N43" s="25">
         <f t="shared" si="0"/>
@@ -8122,16 +8122,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B37"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B32:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update time of sprint 2
</commit_message>
<xml_diff>
--- a/7.Print-Backlog/Sprint-2.xlsx
+++ b/7.Print-Backlog/Sprint-2.xlsx
@@ -525,14 +525,11 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -540,11 +537,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -832,64 +832,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>52</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>52</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -906,11 +906,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="136427008"/>
-        <c:axId val="136428544"/>
+        <c:axId val="180598272"/>
+        <c:axId val="180599808"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="136427008"/>
+        <c:axId val="180598272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,14 +920,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136428544"/>
+        <c:crossAx val="180599808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="136428544"/>
+        <c:axId val="180599808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,7 +938,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="136427008"/>
+        <c:crossAx val="180598272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1494,7 +1494,7 @@
       <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="42" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -1577,7 +1577,7 @@
       <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="37"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="16" t="s">
         <v>20</v>
       </c>
@@ -1658,7 +1658,7 @@
       <c r="A5" s="26">
         <v>4</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="42" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="29" t="s">
@@ -1741,7 +1741,7 @@
       <c r="A6" s="26">
         <v>5</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="13" t="s">
         <v>14</v>
       </c>
@@ -1822,7 +1822,7 @@
       <c r="A7" s="26">
         <v>6</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="42" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -1905,7 +1905,7 @@
       <c r="A8" s="26">
         <v>7</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="13" t="s">
         <v>22</v>
       </c>
@@ -1986,7 +1986,7 @@
       <c r="A9" s="26">
         <v>8</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="13" t="s">
         <v>15</v>
       </c>
@@ -2067,7 +2067,7 @@
       <c r="A10" s="26">
         <v>9</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="42" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -2150,7 +2150,7 @@
       <c r="A11" s="26">
         <v>10</v>
       </c>
-      <c r="B11" s="38"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="13" t="s">
         <v>29</v>
       </c>
@@ -2231,7 +2231,7 @@
       <c r="A12" s="26">
         <v>11</v>
       </c>
-      <c r="B12" s="38"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="17" t="s">
         <v>30</v>
       </c>
@@ -2312,7 +2312,7 @@
       <c r="A13" s="26">
         <v>12</v>
       </c>
-      <c r="B13" s="37"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="17" t="s">
         <v>31</v>
       </c>
@@ -2393,7 +2393,7 @@
       <c r="A14" s="26">
         <v>13</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="42" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -2476,7 +2476,7 @@
       <c r="A15" s="26">
         <v>14</v>
       </c>
-      <c r="B15" s="39"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="13" t="s">
         <v>34</v>
       </c>
@@ -2557,7 +2557,7 @@
       <c r="A16" s="26">
         <v>15</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="13" t="s">
         <v>35</v>
       </c>
@@ -2638,7 +2638,7 @@
       <c r="A17" s="26">
         <v>16</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="36" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -2721,7 +2721,7 @@
       <c r="A18" s="26">
         <v>17</v>
       </c>
-      <c r="B18" s="41"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="13" t="s">
         <v>38</v>
       </c>
@@ -2802,7 +2802,7 @@
       <c r="A19" s="26">
         <v>18</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="13" t="s">
         <v>39</v>
       </c>
@@ -2883,7 +2883,7 @@
       <c r="A20" s="26">
         <v>19</v>
       </c>
-      <c r="B20" s="41"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="12" t="s">
         <v>40</v>
       </c>
@@ -2964,7 +2964,7 @@
       <c r="A21" s="26">
         <v>20</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="36" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -3047,7 +3047,7 @@
       <c r="A22" s="26">
         <v>21</v>
       </c>
-      <c r="B22" s="41"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="13" t="s">
         <v>43</v>
       </c>
@@ -3128,7 +3128,7 @@
       <c r="A23" s="26">
         <v>22</v>
       </c>
-      <c r="B23" s="41"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="13" t="s">
         <v>44</v>
       </c>
@@ -3209,7 +3209,7 @@
       <c r="A24" s="26">
         <v>23</v>
       </c>
-      <c r="B24" s="41"/>
+      <c r="B24" s="36"/>
       <c r="C24" s="12" t="s">
         <v>45</v>
       </c>
@@ -3290,7 +3290,7 @@
       <c r="A25" s="26">
         <v>24</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="36" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -3373,7 +3373,7 @@
       <c r="A26" s="26">
         <v>25</v>
       </c>
-      <c r="B26" s="41"/>
+      <c r="B26" s="36"/>
       <c r="C26" s="13" t="s">
         <v>47</v>
       </c>
@@ -3454,7 +3454,7 @@
       <c r="A27" s="26">
         <v>26</v>
       </c>
-      <c r="B27" s="41"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="13" t="s">
         <v>48</v>
       </c>
@@ -3535,7 +3535,7 @@
       <c r="A28" s="26">
         <v>27</v>
       </c>
-      <c r="B28" s="41"/>
+      <c r="B28" s="36"/>
       <c r="C28" s="12" t="s">
         <v>49</v>
       </c>
@@ -3616,7 +3616,7 @@
       <c r="A29" s="26">
         <v>28</v>
       </c>
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="40" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="13" t="s">
@@ -3699,7 +3699,7 @@
       <c r="A30" s="26">
         <v>29</v>
       </c>
-      <c r="B30" s="38"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="13" t="s">
         <v>58</v>
       </c>
@@ -3780,7 +3780,7 @@
       <c r="A31" s="26">
         <v>30</v>
       </c>
-      <c r="B31" s="37"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="13" t="s">
         <v>59</v>
       </c>
@@ -3861,7 +3861,7 @@
       <c r="A32" s="26">
         <v>31</v>
       </c>
-      <c r="B32" s="42"/>
+      <c r="B32" s="37"/>
       <c r="C32" s="3" t="s">
         <v>50</v>
       </c>
@@ -3942,7 +3942,7 @@
       <c r="A33" s="26">
         <v>32</v>
       </c>
-      <c r="B33" s="39"/>
+      <c r="B33" s="38"/>
       <c r="C33" s="3" t="s">
         <v>51</v>
       </c>
@@ -4023,7 +4023,7 @@
       <c r="A34" s="26">
         <v>33</v>
       </c>
-      <c r="B34" s="39"/>
+      <c r="B34" s="38"/>
       <c r="C34" s="3" t="s">
         <v>52</v>
       </c>
@@ -4104,7 +4104,7 @@
       <c r="A35" s="26">
         <v>34</v>
       </c>
-      <c r="B35" s="39"/>
+      <c r="B35" s="38"/>
       <c r="C35" s="3" t="s">
         <v>53</v>
       </c>
@@ -4185,7 +4185,7 @@
       <c r="A36" s="26">
         <v>35</v>
       </c>
-      <c r="B36" s="39"/>
+      <c r="B36" s="38"/>
       <c r="C36" s="12" t="s">
         <v>54</v>
       </c>
@@ -4266,7 +4266,7 @@
       <c r="A37" s="26">
         <v>36</v>
       </c>
-      <c r="B37" s="40"/>
+      <c r="B37" s="39"/>
       <c r="C37" s="12" t="s">
         <v>60</v>
       </c>
@@ -4767,16 +4767,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B17:B20"/>
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="B25:B28"/>
     <mergeCell ref="B32:B37"/>
     <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4787,8 +4787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43:Z43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4935,13 +4935,13 @@
       <c r="M2" s="23">
         <v>5</v>
       </c>
-      <c r="N2" s="35">
-        <v>0</v>
+      <c r="N2" s="23">
+        <v>5</v>
       </c>
       <c r="O2" s="23">
-        <v>0</v>
-      </c>
-      <c r="P2" s="23">
+        <v>5</v>
+      </c>
+      <c r="P2" s="35">
         <v>0</v>
       </c>
       <c r="Q2" s="23">
@@ -4979,7 +4979,7 @@
       <c r="A3" s="26">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="42" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -5013,13 +5013,13 @@
       <c r="M3" s="23">
         <v>4</v>
       </c>
-      <c r="N3" s="35">
-        <v>0</v>
+      <c r="N3" s="23">
+        <v>4</v>
       </c>
       <c r="O3" s="23">
-        <v>0</v>
-      </c>
-      <c r="P3" s="23">
+        <v>4</v>
+      </c>
+      <c r="P3" s="35">
         <v>0</v>
       </c>
       <c r="Q3" s="23">
@@ -5057,7 +5057,7 @@
       <c r="A4" s="26">
         <v>3</v>
       </c>
-      <c r="B4" s="37"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="16" t="s">
         <v>20</v>
       </c>
@@ -5089,51 +5089,51 @@
       <c r="M4" s="23">
         <v>6</v>
       </c>
-      <c r="N4" s="35">
-        <v>0</v>
+      <c r="N4" s="23">
+        <v>6</v>
       </c>
       <c r="O4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="P4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="S4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="V4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="W4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="X4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Y4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Z4" s="23">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
         <v>4</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="42" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="29" t="s">
@@ -5167,51 +5167,51 @@
       <c r="M5" s="23">
         <v>1</v>
       </c>
-      <c r="N5" s="35">
-        <v>0</v>
+      <c r="N5" s="23">
+        <v>1</v>
       </c>
       <c r="O5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26">
         <v>5</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="13" t="s">
         <v>14</v>
       </c>
@@ -5243,51 +5243,51 @@
       <c r="M6" s="23">
         <v>8</v>
       </c>
-      <c r="N6" s="35">
-        <v>0</v>
+      <c r="N6" s="23">
+        <v>8</v>
       </c>
       <c r="O6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="R6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="V6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="W6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z6" s="23">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26">
         <v>6</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="42" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -5321,51 +5321,51 @@
       <c r="M7" s="23">
         <v>0.5</v>
       </c>
-      <c r="N7" s="35">
-        <v>0</v>
+      <c r="N7" s="23">
+        <v>0.5</v>
       </c>
       <c r="O7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Y7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Z7" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="26">
         <v>7</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="13" t="s">
         <v>22</v>
       </c>
@@ -5397,51 +5397,51 @@
       <c r="M8" s="23">
         <v>1</v>
       </c>
-      <c r="N8" s="35">
-        <v>0</v>
+      <c r="N8" s="23">
+        <v>1</v>
       </c>
       <c r="O8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26">
         <v>8</v>
       </c>
-      <c r="B9" s="37"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="13" t="s">
         <v>15</v>
       </c>
@@ -5473,51 +5473,51 @@
       <c r="M9" s="23">
         <v>1</v>
       </c>
-      <c r="N9" s="35">
-        <v>0</v>
+      <c r="N9" s="23">
+        <v>1</v>
       </c>
       <c r="O9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26">
         <v>9</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="42" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -5551,51 +5551,51 @@
       <c r="M10" s="23">
         <v>0.5</v>
       </c>
-      <c r="N10" s="35">
-        <v>0</v>
+      <c r="N10" s="23">
+        <v>0.5</v>
       </c>
       <c r="O10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Y10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Z10" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26">
         <v>10</v>
       </c>
-      <c r="B11" s="38"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="13" t="s">
         <v>29</v>
       </c>
@@ -5627,51 +5627,51 @@
       <c r="M11" s="23">
         <v>4</v>
       </c>
-      <c r="N11" s="35">
-        <v>0</v>
+      <c r="N11" s="23">
+        <v>4</v>
       </c>
       <c r="O11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z11" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
         <v>11</v>
       </c>
-      <c r="B12" s="38"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="17" t="s">
         <v>30</v>
       </c>
@@ -5703,51 +5703,51 @@
       <c r="M12" s="23">
         <v>2</v>
       </c>
-      <c r="N12" s="35">
-        <v>0</v>
+      <c r="N12" s="23">
+        <v>2</v>
       </c>
       <c r="O12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z12" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26">
         <v>12</v>
       </c>
-      <c r="B13" s="37"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="17" t="s">
         <v>31</v>
       </c>
@@ -5779,51 +5779,51 @@
       <c r="M13" s="23">
         <v>4</v>
       </c>
-      <c r="N13" s="35">
-        <v>0</v>
+      <c r="N13" s="23">
+        <v>4</v>
       </c>
       <c r="O13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z13" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26">
         <v>13</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="42" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -5857,51 +5857,51 @@
       <c r="M14" s="23">
         <v>1</v>
       </c>
-      <c r="N14" s="35">
-        <v>0</v>
+      <c r="N14" s="23">
+        <v>1</v>
       </c>
       <c r="O14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z14" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26">
         <v>14</v>
       </c>
-      <c r="B15" s="39"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="13" t="s">
         <v>34</v>
       </c>
@@ -5933,51 +5933,51 @@
       <c r="M15" s="23">
         <v>2</v>
       </c>
-      <c r="N15" s="35">
-        <v>0</v>
+      <c r="N15" s="23">
+        <v>2</v>
       </c>
       <c r="O15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z15" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26">
         <v>15</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="39"/>
       <c r="C16" s="13" t="s">
         <v>35</v>
       </c>
@@ -6009,51 +6009,51 @@
       <c r="M16" s="23">
         <v>4</v>
       </c>
-      <c r="N16" s="35">
-        <v>0</v>
+      <c r="N16" s="23">
+        <v>4</v>
       </c>
       <c r="O16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z16" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:26" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26">
         <v>16</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="36" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="13" t="s">
@@ -6087,51 +6087,51 @@
       <c r="M17" s="23">
         <v>1</v>
       </c>
-      <c r="N17" s="35">
-        <v>0</v>
+      <c r="N17" s="23">
+        <v>1</v>
       </c>
       <c r="O17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z17" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:26" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26">
         <v>17</v>
       </c>
-      <c r="B18" s="41"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="13" t="s">
         <v>38</v>
       </c>
@@ -6163,51 +6163,51 @@
       <c r="M18" s="23">
         <v>2</v>
       </c>
-      <c r="N18" s="35">
-        <v>0</v>
+      <c r="N18" s="23">
+        <v>2</v>
       </c>
       <c r="O18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z18" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="26">
         <v>18</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="13" t="s">
         <v>39</v>
       </c>
@@ -6239,51 +6239,51 @@
       <c r="M19" s="23">
         <v>2</v>
       </c>
-      <c r="N19" s="35">
-        <v>0</v>
+      <c r="N19" s="23">
+        <v>2</v>
       </c>
       <c r="O19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z19" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26">
         <v>19</v>
       </c>
-      <c r="B20" s="41"/>
+      <c r="B20" s="36"/>
       <c r="C20" s="12" t="s">
         <v>40</v>
       </c>
@@ -6315,51 +6315,51 @@
       <c r="M20" s="23">
         <v>5</v>
       </c>
-      <c r="N20" s="35">
-        <v>0</v>
+      <c r="N20" s="23">
+        <v>5</v>
       </c>
       <c r="O20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Z20" s="23">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="26">
         <v>20</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="36" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -6393,51 +6393,51 @@
       <c r="M21" s="23">
         <v>1</v>
       </c>
-      <c r="N21" s="35">
-        <v>0</v>
+      <c r="N21" s="23">
+        <v>1</v>
       </c>
       <c r="O21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z21" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="26">
         <v>21</v>
       </c>
-      <c r="B22" s="41"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="13" t="s">
         <v>43</v>
       </c>
@@ -6469,51 +6469,51 @@
       <c r="M22" s="23">
         <v>1</v>
       </c>
-      <c r="N22" s="35">
-        <v>0</v>
+      <c r="N22" s="23">
+        <v>1</v>
       </c>
       <c r="O22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z22" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="26">
         <v>22</v>
       </c>
-      <c r="B23" s="41"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="13" t="s">
         <v>44</v>
       </c>
@@ -6545,51 +6545,51 @@
       <c r="M23" s="23">
         <v>2</v>
       </c>
-      <c r="N23" s="35">
-        <v>0</v>
+      <c r="N23" s="23">
+        <v>2</v>
       </c>
       <c r="O23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z23" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26">
         <v>23</v>
       </c>
-      <c r="B24" s="41"/>
+      <c r="B24" s="36"/>
       <c r="C24" s="12" t="s">
         <v>45</v>
       </c>
@@ -6621,51 +6621,51 @@
       <c r="M24" s="23">
         <v>2</v>
       </c>
-      <c r="N24" s="35">
-        <v>0</v>
+      <c r="N24" s="23">
+        <v>2</v>
       </c>
       <c r="O24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z24" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26">
         <v>24</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="36" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -6699,51 +6699,51 @@
       <c r="M25" s="23">
         <v>0.5</v>
       </c>
-      <c r="N25" s="35">
-        <v>0</v>
+      <c r="N25" s="23">
+        <v>0.5</v>
       </c>
       <c r="O25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Y25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Z25" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="26">
         <v>25</v>
       </c>
-      <c r="B26" s="41"/>
+      <c r="B26" s="36"/>
       <c r="C26" s="13" t="s">
         <v>47</v>
       </c>
@@ -6775,51 +6775,51 @@
       <c r="M26" s="23">
         <v>1</v>
       </c>
-      <c r="N26" s="35">
-        <v>0</v>
+      <c r="N26" s="23">
+        <v>1</v>
       </c>
       <c r="O26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z26" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="26">
         <v>26</v>
       </c>
-      <c r="B27" s="41"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="13" t="s">
         <v>48</v>
       </c>
@@ -6851,51 +6851,51 @@
       <c r="M27" s="23">
         <v>2</v>
       </c>
-      <c r="N27" s="35">
-        <v>0</v>
+      <c r="N27" s="23">
+        <v>2</v>
       </c>
       <c r="O27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z27" s="23">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26">
         <v>27</v>
       </c>
-      <c r="B28" s="41"/>
+      <c r="B28" s="36"/>
       <c r="C28" s="12" t="s">
         <v>49</v>
       </c>
@@ -6927,51 +6927,51 @@
       <c r="M28" s="23">
         <v>4</v>
       </c>
-      <c r="N28" s="35">
-        <v>0</v>
+      <c r="N28" s="23">
+        <v>4</v>
       </c>
       <c r="O28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z28" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:26" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="26">
         <v>28</v>
       </c>
-      <c r="B29" s="38" t="s">
+      <c r="B29" s="40" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="13" t="s">
@@ -7005,51 +7005,51 @@
       <c r="M29" s="23">
         <v>0.5</v>
       </c>
-      <c r="N29" s="35">
-        <v>0</v>
+      <c r="N29" s="23">
+        <v>0.5</v>
       </c>
       <c r="O29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Y29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Z29" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:26" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="26">
         <v>29</v>
       </c>
-      <c r="B30" s="38"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="13" t="s">
         <v>58</v>
       </c>
@@ -7081,51 +7081,51 @@
       <c r="M30" s="23">
         <v>1</v>
       </c>
-      <c r="N30" s="35">
-        <v>0</v>
+      <c r="N30" s="23">
+        <v>1</v>
       </c>
       <c r="O30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z30" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:26" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="26">
         <v>30</v>
       </c>
-      <c r="B31" s="37"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="13" t="s">
         <v>59</v>
       </c>
@@ -7157,51 +7157,51 @@
       <c r="M31" s="23">
         <v>4</v>
       </c>
-      <c r="N31" s="35">
-        <v>0</v>
+      <c r="N31" s="23">
+        <v>4</v>
       </c>
       <c r="O31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z31" s="23">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:26" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26">
         <v>31</v>
       </c>
-      <c r="B32" s="42"/>
+      <c r="B32" s="37"/>
       <c r="C32" s="3" t="s">
         <v>50</v>
       </c>
@@ -7233,51 +7233,51 @@
       <c r="M32" s="23">
         <v>0.5</v>
       </c>
-      <c r="N32" s="35">
-        <v>0</v>
+      <c r="N32" s="23">
+        <v>0.5</v>
       </c>
       <c r="O32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Y32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Z32" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="26">
         <v>32</v>
       </c>
-      <c r="B33" s="39"/>
+      <c r="B33" s="38"/>
       <c r="C33" s="3" t="s">
         <v>51</v>
       </c>
@@ -7309,51 +7309,51 @@
       <c r="M33" s="23">
         <v>0.5</v>
       </c>
-      <c r="N33" s="35">
-        <v>0</v>
+      <c r="N33" s="23">
+        <v>0.5</v>
       </c>
       <c r="O33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Y33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Z33" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26">
         <v>33</v>
       </c>
-      <c r="B34" s="39"/>
+      <c r="B34" s="38"/>
       <c r="C34" s="3" t="s">
         <v>52</v>
       </c>
@@ -7385,51 +7385,51 @@
       <c r="M34" s="23">
         <v>0.5</v>
       </c>
-      <c r="N34" s="35">
-        <v>0</v>
+      <c r="N34" s="23">
+        <v>0.5</v>
       </c>
       <c r="O34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Y34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Z34" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="26">
         <v>34</v>
       </c>
-      <c r="B35" s="39"/>
+      <c r="B35" s="38"/>
       <c r="C35" s="3" t="s">
         <v>53</v>
       </c>
@@ -7461,51 +7461,51 @@
       <c r="M35" s="23">
         <v>0.5</v>
       </c>
-      <c r="N35" s="35">
-        <v>0</v>
+      <c r="N35" s="23">
+        <v>0.5</v>
       </c>
       <c r="O35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Y35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Z35" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26">
         <v>35</v>
       </c>
-      <c r="B36" s="39"/>
+      <c r="B36" s="38"/>
       <c r="C36" s="12" t="s">
         <v>54</v>
       </c>
@@ -7537,51 +7537,51 @@
       <c r="M36" s="23">
         <v>0.5</v>
       </c>
-      <c r="N36" s="35">
-        <v>0</v>
+      <c r="N36" s="23">
+        <v>0.5</v>
       </c>
       <c r="O36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Y36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Z36" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="26">
         <v>36</v>
       </c>
-      <c r="B37" s="40"/>
+      <c r="B37" s="39"/>
       <c r="C37" s="12" t="s">
         <v>60</v>
       </c>
@@ -7613,44 +7613,44 @@
       <c r="M37" s="23">
         <v>0.5</v>
       </c>
-      <c r="N37" s="35">
-        <v>0</v>
+      <c r="N37" s="23">
+        <v>0.5</v>
       </c>
       <c r="O37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="U37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="X37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Y37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Z37" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="38" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8040,98 +8040,98 @@
         <v>4</v>
       </c>
       <c r="G43" s="25">
-        <f>SUM(G7:G41)</f>
-        <v>52</v>
+        <f>SUM(G2:G37)</f>
+        <v>76</v>
       </c>
       <c r="H43" s="25">
-        <f t="shared" ref="H43:Z43" si="0">SUM(H7:H41)</f>
-        <v>52</v>
+        <f t="shared" ref="H43:Z43" si="0">SUM(H2:H37)</f>
+        <v>76</v>
       </c>
       <c r="I43" s="25">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="J43" s="25">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="K43" s="25">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="L43" s="25">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="M43" s="25">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="N43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="O43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="P43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="Q43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="R43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="S43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="T43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="U43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="V43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="W43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="X43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="Y43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="Z43" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B17:B20"/>
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="B25:B28"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B32:B37"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>